<commit_message>
- Renamed options 'template' --> 'style' and 'preset' --> 'template'. - Added handling for 'hidden' (for JHU Collect specific Android client app case) and other custom types. - Added abstract class around calculate and custom types. - Various refactorings. - Continued work around relevant --> question number implementation.
</commit_message>
<xml_diff>
--- a/test/static/multiple_file_language_option_conversion/BFR5-Female-Questionnaire-v13-jef.xlsx
+++ b/test/static/multiple_file_language_option_conversion/BFR5-Female-Questionnaire-v13-jef.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26460" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26460"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -13942,14 +13942,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR578"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D314" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B317" sqref="B317"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.5" style="75" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" style="75" customWidth="1"/>
@@ -13979,7 +13979,7 @@
     <col min="26" max="16384" width="8.6640625" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="28">
+    <row r="1" spans="1:25" ht="13" customHeight="1">
       <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
@@ -14054,7 +14054,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" ht="13" customHeight="1">
       <c r="A2" s="73" t="s">
         <v>14</v>
       </c>
@@ -14088,7 +14088,7 @@
       </c>
       <c r="U2" s="75"/>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" ht="13" customHeight="1">
       <c r="A3" s="73" t="s">
         <v>16</v>
       </c>
@@ -14125,7 +14125,7 @@
       </c>
       <c r="U3" s="75"/>
     </row>
-    <row r="4" spans="1:25" ht="112">
+    <row r="4" spans="1:25" ht="13" customHeight="1">
       <c r="A4" s="73" t="s">
         <v>20</v>
       </c>
@@ -14162,7 +14162,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" ht="13" customHeight="1">
       <c r="A5" s="73" t="s">
         <v>22</v>
       </c>
@@ -14201,7 +14201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" ht="13" customHeight="1">
       <c r="A6" s="73" t="s">
         <v>27</v>
       </c>
@@ -14233,7 +14233,7 @@
       </c>
       <c r="U6" s="75"/>
     </row>
-    <row r="7" spans="1:25" ht="42">
+    <row r="7" spans="1:25" ht="13" customHeight="1">
       <c r="A7" s="73" t="s">
         <v>28</v>
       </c>
@@ -14275,7 +14275,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="42">
+    <row r="8" spans="1:25" ht="13" customHeight="1">
       <c r="A8" s="73" t="s">
         <v>32</v>
       </c>
@@ -14319,7 +14319,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="56">
+    <row r="9" spans="1:25" ht="13" customHeight="1">
       <c r="A9" s="73" t="s">
         <v>37</v>
       </c>
@@ -14363,7 +14363,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="56">
+    <row r="10" spans="1:25" ht="13" customHeight="1">
       <c r="A10" s="73" t="s">
         <v>16</v>
       </c>
@@ -14404,7 +14404,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="131" customFormat="1">
+    <row r="11" spans="1:25" s="131" customFormat="1" ht="13" customHeight="1">
       <c r="A11" s="131" t="s">
         <v>37</v>
       </c>
@@ -14434,7 +14434,7 @@
       </c>
       <c r="W11"/>
     </row>
-    <row r="12" spans="1:25" s="131" customFormat="1">
+    <row r="12" spans="1:25" s="131" customFormat="1" ht="13" customHeight="1">
       <c r="A12" s="131" t="s">
         <v>37</v>
       </c>
@@ -14464,7 +14464,7 @@
       </c>
       <c r="W12"/>
     </row>
-    <row r="13" spans="1:25" s="131" customFormat="1">
+    <row r="13" spans="1:25" s="131" customFormat="1" ht="13" customHeight="1">
       <c r="A13" s="131" t="s">
         <v>37</v>
       </c>
@@ -14494,7 +14494,7 @@
       </c>
       <c r="W13"/>
     </row>
-    <row r="14" spans="1:25" s="78" customFormat="1">
+    <row r="14" spans="1:25" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A14" s="77" t="s">
         <v>37</v>
       </c>
@@ -14534,7 +14534,7 @@
       <c r="X14" s="77"/>
       <c r="Y14" s="77"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" ht="13" customHeight="1">
       <c r="A15" s="73" t="s">
         <v>46</v>
       </c>
@@ -14575,7 +14575,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" ht="13" customHeight="1">
       <c r="A16" s="73" t="s">
         <v>46</v>
       </c>
@@ -14616,7 +14616,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" ht="13" customHeight="1">
       <c r="A17" s="73" t="s">
         <v>27</v>
       </c>
@@ -14648,7 +14648,7 @@
       </c>
       <c r="U17" s="75"/>
     </row>
-    <row r="18" spans="1:25" s="78" customFormat="1" ht="98">
+    <row r="18" spans="1:25" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A18" s="77" t="s">
         <v>14</v>
       </c>
@@ -14684,7 +14684,7 @@
       <c r="X18" s="77"/>
       <c r="Y18" s="77"/>
     </row>
-    <row r="19" spans="1:25" ht="154">
+    <row r="19" spans="1:25" ht="13" customHeight="1">
       <c r="A19" s="73" t="s">
         <v>28</v>
       </c>
@@ -14738,7 +14738,7 @@
       </c>
       <c r="Y19" s="75"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" ht="13" customHeight="1">
       <c r="A20" s="73" t="s">
         <v>16</v>
       </c>
@@ -14772,7 +14772,7 @@
       </c>
       <c r="U20" s="75"/>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" ht="13" customHeight="1">
       <c r="A21" s="73" t="s">
         <v>37</v>
       </c>
@@ -14817,7 +14817,7 @@
         <v>2428</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="28">
+    <row r="22" spans="1:25" ht="13" customHeight="1">
       <c r="A22" s="73" t="s">
         <v>28</v>
       </c>
@@ -14858,7 +14858,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" ht="13" customHeight="1">
       <c r="A23" s="73" t="s">
         <v>27</v>
       </c>
@@ -14890,7 +14890,7 @@
       </c>
       <c r="U23" s="75"/>
     </row>
-    <row r="24" spans="1:25" ht="42">
+    <row r="24" spans="1:25" ht="13" customHeight="1">
       <c r="A24" s="73" t="s">
         <v>37</v>
       </c>
@@ -14941,7 +14941,7 @@
         <v>2431</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="42">
+    <row r="25" spans="1:25" ht="13" customHeight="1">
       <c r="A25" s="73" t="s">
         <v>16</v>
       </c>
@@ -14978,7 +14978,7 @@
       </c>
       <c r="U25" s="75"/>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" ht="13" customHeight="1">
       <c r="A26" s="73" t="s">
         <v>65</v>
       </c>
@@ -15023,7 +15023,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="28">
+    <row r="27" spans="1:25" ht="13" customHeight="1">
       <c r="A27" s="73" t="s">
         <v>28</v>
       </c>
@@ -15062,7 +15062,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" ht="13" customHeight="1">
       <c r="A28" s="73" t="s">
         <v>27</v>
       </c>
@@ -15094,7 +15094,7 @@
       </c>
       <c r="U28" s="75"/>
     </row>
-    <row r="29" spans="1:25" s="78" customFormat="1" ht="70">
+    <row r="29" spans="1:25" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A29" s="77" t="s">
         <v>65</v>
       </c>
@@ -15150,7 +15150,7 @@
       </c>
       <c r="Y29" s="77"/>
     </row>
-    <row r="30" spans="1:25" ht="42">
+    <row r="30" spans="1:25" ht="13" customHeight="1">
       <c r="A30" s="73" t="s">
         <v>14</v>
       </c>
@@ -15184,7 +15184,7 @@
       </c>
       <c r="U30" s="75"/>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" ht="13" customHeight="1">
       <c r="A31" s="73" t="s">
         <v>16</v>
       </c>
@@ -15216,7 +15216,7 @@
       </c>
       <c r="U31" s="75"/>
     </row>
-    <row r="32" spans="1:25" s="78" customFormat="1" ht="70">
+    <row r="32" spans="1:25" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A32" s="77" t="s">
         <v>20</v>
       </c>
@@ -15260,7 +15260,7 @@
       <c r="X32" s="77"/>
       <c r="Y32" s="77"/>
     </row>
-    <row r="33" spans="1:28" s="78" customFormat="1" ht="42">
+    <row r="33" spans="1:28" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A33" s="77" t="s">
         <v>20</v>
       </c>
@@ -15304,7 +15304,7 @@
       <c r="X33" s="77"/>
       <c r="Y33" s="77"/>
     </row>
-    <row r="34" spans="1:28" s="131" customFormat="1">
+    <row r="34" spans="1:28" s="131" customFormat="1" ht="13" customHeight="1">
       <c r="A34" s="131" t="s">
         <v>37</v>
       </c>
@@ -15329,7 +15329,7 @@
         <v>2433</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="131" customFormat="1">
+    <row r="35" spans="1:28" s="131" customFormat="1" ht="13" customHeight="1">
       <c r="A35" s="131" t="s">
         <v>37</v>
       </c>
@@ -15354,7 +15354,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="36" spans="1:28" s="131" customFormat="1">
+    <row r="36" spans="1:28" s="131" customFormat="1" ht="13" customHeight="1">
       <c r="A36" s="131" t="s">
         <v>37</v>
       </c>
@@ -15379,7 +15379,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="78" customFormat="1" ht="28">
+    <row r="37" spans="1:28" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A37" s="77" t="s">
         <v>37</v>
       </c>
@@ -15417,7 +15417,7 @@
       <c r="X37" s="77"/>
       <c r="Y37" s="77"/>
     </row>
-    <row r="38" spans="1:28" s="78" customFormat="1" ht="28">
+    <row r="38" spans="1:28" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A38" s="77" t="s">
         <v>46</v>
       </c>
@@ -15455,7 +15455,7 @@
       <c r="X38" s="77"/>
       <c r="Y38" s="77"/>
     </row>
-    <row r="39" spans="1:28" s="78" customFormat="1" ht="28">
+    <row r="39" spans="1:28" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A39" s="77" t="s">
         <v>46</v>
       </c>
@@ -15493,7 +15493,7 @@
       <c r="X39" s="77"/>
       <c r="Y39" s="77"/>
     </row>
-    <row r="40" spans="1:28" ht="28">
+    <row r="40" spans="1:28" ht="13" customHeight="1">
       <c r="A40" s="73" t="s">
         <v>28</v>
       </c>
@@ -15537,7 +15537,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:28">
+    <row r="41" spans="1:28" ht="13" customHeight="1">
       <c r="A41" s="73" t="s">
         <v>27</v>
       </c>
@@ -15569,7 +15569,7 @@
       </c>
       <c r="U41" s="75"/>
     </row>
-    <row r="42" spans="1:28" ht="409">
+    <row r="42" spans="1:28" ht="13" customHeight="1">
       <c r="A42" s="73" t="s">
         <v>28</v>
       </c>
@@ -15625,7 +15625,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="42">
+    <row r="43" spans="1:28" ht="13" customHeight="1">
       <c r="A43" s="73" t="s">
         <v>28</v>
       </c>
@@ -15666,7 +15666,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="56">
+    <row r="44" spans="1:28" ht="13" customHeight="1">
       <c r="A44" s="73" t="s">
         <v>92</v>
       </c>
@@ -15710,7 +15710,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="79" customFormat="1" ht="70">
+    <row r="45" spans="1:28" s="79" customFormat="1" ht="13" customHeight="1">
       <c r="A45" s="79" t="s">
         <v>162</v>
       </c>
@@ -15745,7 +15745,7 @@
       <c r="AA45" s="81"/>
       <c r="AB45" s="81"/>
     </row>
-    <row r="46" spans="1:28" s="78" customFormat="1" ht="252">
+    <row r="46" spans="1:28" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A46" s="77" t="s">
         <v>20</v>
       </c>
@@ -15795,7 +15795,7 @@
       <c r="X46" s="77"/>
       <c r="Y46" s="77"/>
     </row>
-    <row r="47" spans="1:28" s="78" customFormat="1" ht="409">
+    <row r="47" spans="1:28" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A47" s="77" t="s">
         <v>20</v>
       </c>
@@ -15841,7 +15841,7 @@
       <c r="X47" s="77"/>
       <c r="Y47" s="77"/>
     </row>
-    <row r="48" spans="1:28" s="78" customFormat="1" ht="70">
+    <row r="48" spans="1:28" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A48" s="78" t="s">
         <v>28</v>
       </c>
@@ -15875,7 +15875,7 @@
       <c r="X48" s="77"/>
       <c r="Y48" s="77"/>
     </row>
-    <row r="49" spans="1:49" s="78" customFormat="1" ht="28">
+    <row r="49" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A49" s="78" t="s">
         <v>16</v>
       </c>
@@ -15904,7 +15904,7 @@
       <c r="X49" s="77"/>
       <c r="Y49" s="77"/>
     </row>
-    <row r="50" spans="1:49" s="78" customFormat="1">
+    <row r="50" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A50" s="78" t="s">
         <v>32</v>
       </c>
@@ -15936,7 +15936,7 @@
       <c r="X50" s="77"/>
       <c r="Y50" s="77"/>
     </row>
-    <row r="51" spans="1:49" s="78" customFormat="1" ht="28">
+    <row r="51" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A51" s="78" t="s">
         <v>104</v>
       </c>
@@ -15962,7 +15962,7 @@
       <c r="X51" s="77"/>
       <c r="Y51" s="77"/>
     </row>
-    <row r="52" spans="1:49" s="78" customFormat="1">
+    <row r="52" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A52" s="78" t="s">
         <v>27</v>
       </c>
@@ -15984,7 +15984,7 @@
       <c r="X52" s="77"/>
       <c r="Y52" s="77"/>
     </row>
-    <row r="53" spans="1:49" s="78" customFormat="1" ht="42">
+    <row r="53" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A53" s="78" t="s">
         <v>14</v>
       </c>
@@ -16009,7 +16009,7 @@
       <c r="X53" s="77"/>
       <c r="Y53" s="77"/>
     </row>
-    <row r="54" spans="1:49" s="78" customFormat="1" ht="210">
+    <row r="54" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A54" s="77" t="s">
         <v>20</v>
       </c>
@@ -16055,7 +16055,7 @@
       <c r="X54" s="77"/>
       <c r="Y54" s="77"/>
     </row>
-    <row r="55" spans="1:49" ht="70">
+    <row r="55" spans="1:49" ht="13" customHeight="1">
       <c r="A55" s="73" t="s">
         <v>104</v>
       </c>
@@ -16107,7 +16107,7 @@
       </c>
       <c r="X55" s="131"/>
     </row>
-    <row r="56" spans="1:49" ht="126">
+    <row r="56" spans="1:49" ht="13" customHeight="1">
       <c r="A56" s="73" t="s">
         <v>37</v>
       </c>
@@ -16159,7 +16159,7 @@
         <v>2434</v>
       </c>
     </row>
-    <row r="57" spans="1:49" ht="182">
+    <row r="57" spans="1:49" ht="13" customHeight="1">
       <c r="A57" s="73" t="s">
         <v>37</v>
       </c>
@@ -16208,7 +16208,7 @@
       </c>
       <c r="X57" s="131"/>
     </row>
-    <row r="58" spans="1:49">
+    <row r="58" spans="1:49" ht="13" customHeight="1">
       <c r="A58" s="73" t="s">
         <v>14</v>
       </c>
@@ -16242,7 +16242,7 @@
       </c>
       <c r="U58" s="75"/>
     </row>
-    <row r="59" spans="1:49" s="85" customFormat="1" ht="112">
+    <row r="59" spans="1:49" s="85" customFormat="1" ht="13" customHeight="1">
       <c r="A59" s="84" t="s">
         <v>20</v>
       </c>
@@ -16292,7 +16292,7 @@
       <c r="X59" s="84"/>
       <c r="Y59" s="84"/>
     </row>
-    <row r="60" spans="1:49" s="86" customFormat="1">
+    <row r="60" spans="1:49" s="86" customFormat="1" ht="13" customHeight="1">
       <c r="A60" s="86" t="s">
         <v>16</v>
       </c>
@@ -16322,7 +16322,7 @@
       <c r="X60" s="75"/>
       <c r="Y60" s="75"/>
     </row>
-    <row r="61" spans="1:49" s="78" customFormat="1" ht="70">
+    <row r="61" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A61" s="77" t="s">
         <v>20</v>
       </c>
@@ -16386,7 +16386,7 @@
       <c r="AV61" s="77"/>
       <c r="AW61" s="77"/>
     </row>
-    <row r="62" spans="1:49" s="78" customFormat="1" ht="42">
+    <row r="62" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A62" s="77" t="s">
         <v>20</v>
       </c>
@@ -16450,7 +16450,7 @@
       <c r="AV62" s="77"/>
       <c r="AW62" s="77"/>
     </row>
-    <row r="63" spans="1:49" s="89" customFormat="1" ht="28">
+    <row r="63" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A63" s="86" t="s">
         <v>1665</v>
       </c>
@@ -16495,7 +16495,7 @@
       <c r="AS63" s="86"/>
       <c r="AT63" s="86"/>
     </row>
-    <row r="64" spans="1:49" s="89" customFormat="1">
+    <row r="64" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A64" s="86" t="s">
         <v>122</v>
       </c>
@@ -16544,7 +16544,7 @@
       <c r="AS64" s="86"/>
       <c r="AT64" s="86"/>
     </row>
-    <row r="65" spans="1:70" s="89" customFormat="1" ht="84">
+    <row r="65" spans="1:70" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A65" s="86" t="s">
         <v>14</v>
       </c>
@@ -16585,7 +16585,7 @@
       <c r="AS65" s="91"/>
       <c r="AT65" s="86"/>
     </row>
-    <row r="66" spans="1:70" s="89" customFormat="1" ht="28">
+    <row r="66" spans="1:70" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A66" s="86" t="s">
         <v>14</v>
       </c>
@@ -16626,7 +16626,7 @@
       <c r="AS66" s="91"/>
       <c r="AT66" s="86"/>
     </row>
-    <row r="67" spans="1:70" s="86" customFormat="1">
+    <row r="67" spans="1:70" s="86" customFormat="1" ht="13" customHeight="1">
       <c r="A67" s="86" t="s">
         <v>27</v>
       </c>
@@ -16648,7 +16648,7 @@
       <c r="X67" s="75"/>
       <c r="Y67" s="75"/>
     </row>
-    <row r="68" spans="1:70" ht="28">
+    <row r="68" spans="1:70" ht="13" customHeight="1">
       <c r="A68" s="73" t="s">
         <v>14</v>
       </c>
@@ -16682,7 +16682,7 @@
       </c>
       <c r="U68" s="75"/>
     </row>
-    <row r="69" spans="1:70" ht="28">
+    <row r="69" spans="1:70" ht="13" customHeight="1">
       <c r="A69" s="73" t="s">
         <v>14</v>
       </c>
@@ -16716,7 +16716,7 @@
       </c>
       <c r="U69" s="75"/>
     </row>
-    <row r="70" spans="1:70" ht="70">
+    <row r="70" spans="1:70" ht="13" customHeight="1">
       <c r="A70" s="73" t="s">
         <v>14</v>
       </c>
@@ -16750,7 +16750,7 @@
       </c>
       <c r="U70" s="75"/>
     </row>
-    <row r="71" spans="1:70" ht="70">
+    <row r="71" spans="1:70" ht="13" customHeight="1">
       <c r="A71" s="73" t="s">
         <v>14</v>
       </c>
@@ -16784,7 +16784,7 @@
       </c>
       <c r="U71" s="75"/>
     </row>
-    <row r="72" spans="1:70" ht="140">
+    <row r="72" spans="1:70" ht="13" customHeight="1">
       <c r="A72" s="73" t="s">
         <v>46</v>
       </c>
@@ -16835,7 +16835,7 @@
         <v>2682</v>
       </c>
     </row>
-    <row r="73" spans="1:70" s="74" customFormat="1">
+    <row r="73" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A73" s="73" t="s">
         <v>16</v>
       </c>
@@ -16923,7 +16923,7 @@
       <c r="BQ73" s="75"/>
       <c r="BR73" s="75"/>
     </row>
-    <row r="74" spans="1:70" s="74" customFormat="1" ht="238">
+    <row r="74" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A74" s="73" t="s">
         <v>20</v>
       </c>
@@ -17011,7 +17011,7 @@
       <c r="BQ74" s="75"/>
       <c r="BR74" s="75"/>
     </row>
-    <row r="75" spans="1:70" s="74" customFormat="1" ht="140">
+    <row r="75" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A75" s="73" t="s">
         <v>20</v>
       </c>
@@ -17099,7 +17099,7 @@
       <c r="BQ75" s="75"/>
       <c r="BR75" s="75"/>
     </row>
-    <row r="76" spans="1:70" s="74" customFormat="1" ht="56">
+    <row r="76" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A76" s="73" t="s">
         <v>20</v>
       </c>
@@ -17187,7 +17187,7 @@
       <c r="BQ76" s="75"/>
       <c r="BR76" s="75"/>
     </row>
-    <row r="77" spans="1:70" s="74" customFormat="1" ht="28">
+    <row r="77" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A77" s="73" t="s">
         <v>46</v>
       </c>
@@ -17281,7 +17281,7 @@
       <c r="BQ77" s="75"/>
       <c r="BR77" s="75"/>
     </row>
-    <row r="78" spans="1:70" s="74" customFormat="1">
+    <row r="78" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A78" s="73" t="s">
         <v>27</v>
       </c>
@@ -17363,7 +17363,7 @@
       <c r="BQ78" s="75"/>
       <c r="BR78" s="75"/>
     </row>
-    <row r="79" spans="1:70" s="78" customFormat="1" ht="126">
+    <row r="79" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A79" s="77" t="s">
         <v>137</v>
       </c>
@@ -17413,7 +17413,7 @@
       <c r="X79" s="77"/>
       <c r="Y79" s="77"/>
     </row>
-    <row r="80" spans="1:70" ht="98">
+    <row r="80" spans="1:70" ht="13" customHeight="1">
       <c r="A80" s="73" t="s">
         <v>139</v>
       </c>
@@ -17462,7 +17462,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="81" spans="1:46" ht="42">
+    <row r="81" spans="1:46" ht="13" customHeight="1">
       <c r="A81" s="73" t="s">
         <v>141</v>
       </c>
@@ -17506,7 +17506,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="82" spans="1:46" s="89" customFormat="1" ht="28">
+    <row r="82" spans="1:46" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A82" s="86" t="s">
         <v>16</v>
       </c>
@@ -17553,7 +17553,7 @@
       <c r="AS82" s="86"/>
       <c r="AT82" s="86"/>
     </row>
-    <row r="83" spans="1:46" ht="120">
+    <row r="83" spans="1:46" ht="13" customHeight="1">
       <c r="A83" s="73" t="s">
         <v>20</v>
       </c>
@@ -17604,7 +17604,7 @@
       <c r="AS83" s="73"/>
       <c r="AT83" s="73"/>
     </row>
-    <row r="84" spans="1:46" s="89" customFormat="1" ht="28">
+    <row r="84" spans="1:46" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A84" s="86" t="s">
         <v>1665</v>
       </c>
@@ -17649,7 +17649,7 @@
       <c r="AS84" s="86"/>
       <c r="AT84" s="86"/>
     </row>
-    <row r="85" spans="1:46" s="89" customFormat="1" ht="42">
+    <row r="85" spans="1:46" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A85" s="86" t="s">
         <v>122</v>
       </c>
@@ -17702,7 +17702,7 @@
       <c r="AS85" s="86"/>
       <c r="AT85" s="86"/>
     </row>
-    <row r="86" spans="1:46" s="89" customFormat="1">
+    <row r="86" spans="1:46" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A86" s="86" t="s">
         <v>14</v>
       </c>
@@ -17743,7 +17743,7 @@
       <c r="AS86" s="86"/>
       <c r="AT86" s="86"/>
     </row>
-    <row r="87" spans="1:46" s="89" customFormat="1" ht="70">
+    <row r="87" spans="1:46" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A87" s="86" t="s">
         <v>14</v>
       </c>
@@ -17784,7 +17784,7 @@
       <c r="AS87" s="86"/>
       <c r="AT87" s="86"/>
     </row>
-    <row r="88" spans="1:46" s="89" customFormat="1" ht="42">
+    <row r="88" spans="1:46" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A88" s="86" t="s">
         <v>14</v>
       </c>
@@ -17825,7 +17825,7 @@
       <c r="AS88" s="86"/>
       <c r="AT88" s="86"/>
     </row>
-    <row r="89" spans="1:46" s="89" customFormat="1">
+    <row r="89" spans="1:46" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A89" s="86" t="s">
         <v>27</v>
       </c>
@@ -17864,7 +17864,7 @@
       <c r="AS89" s="86"/>
       <c r="AT89" s="86"/>
     </row>
-    <row r="90" spans="1:46" s="94" customFormat="1" ht="98">
+    <row r="90" spans="1:46" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A90" s="86" t="s">
         <v>20</v>
       </c>
@@ -17906,7 +17906,7 @@
       <c r="X90" s="75"/>
       <c r="Y90" s="75"/>
     </row>
-    <row r="91" spans="1:46" s="89" customFormat="1" ht="126">
+    <row r="91" spans="1:46" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A91" s="86" t="s">
         <v>20</v>
       </c>
@@ -17953,7 +17953,7 @@
       <c r="AS91" s="86"/>
       <c r="AT91" s="86"/>
     </row>
-    <row r="92" spans="1:46" s="89" customFormat="1" ht="168">
+    <row r="92" spans="1:46" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A92" s="86" t="s">
         <v>20</v>
       </c>
@@ -18000,7 +18000,7 @@
       <c r="AS92" s="86"/>
       <c r="AT92" s="86"/>
     </row>
-    <row r="93" spans="1:46" ht="42">
+    <row r="93" spans="1:46" ht="13" customHeight="1">
       <c r="A93" s="73" t="s">
         <v>14</v>
       </c>
@@ -18037,7 +18037,7 @@
       </c>
       <c r="U93" s="75"/>
     </row>
-    <row r="94" spans="1:46" ht="42">
+    <row r="94" spans="1:46" ht="13" customHeight="1">
       <c r="A94" s="73" t="s">
         <v>14</v>
       </c>
@@ -18074,7 +18074,7 @@
       </c>
       <c r="U94" s="75"/>
     </row>
-    <row r="95" spans="1:46" ht="168">
+    <row r="95" spans="1:46" ht="13" customHeight="1">
       <c r="A95" s="73" t="s">
         <v>14</v>
       </c>
@@ -18111,7 +18111,7 @@
       </c>
       <c r="U95" s="75"/>
     </row>
-    <row r="96" spans="1:46" ht="98">
+    <row r="96" spans="1:46" ht="13" customHeight="1">
       <c r="A96" s="73" t="s">
         <v>28</v>
       </c>
@@ -18157,7 +18157,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="97" spans="1:49" s="89" customFormat="1" ht="56">
+    <row r="97" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A97" s="86" t="s">
         <v>16</v>
       </c>
@@ -18204,7 +18204,7 @@
       <c r="AS97" s="86"/>
       <c r="AT97" s="86"/>
     </row>
-    <row r="98" spans="1:49" s="78" customFormat="1" ht="120">
+    <row r="98" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A98" s="77" t="s">
         <v>20</v>
       </c>
@@ -18266,7 +18266,7 @@
       <c r="AV98" s="77"/>
       <c r="AW98" s="77"/>
     </row>
-    <row r="99" spans="1:49" s="89" customFormat="1" ht="28">
+    <row r="99" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A99" s="86" t="s">
         <v>1665</v>
       </c>
@@ -18311,7 +18311,7 @@
       <c r="AS99" s="86"/>
       <c r="AT99" s="86"/>
     </row>
-    <row r="100" spans="1:49" s="89" customFormat="1" ht="42">
+    <row r="100" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A100" s="86" t="s">
         <v>122</v>
       </c>
@@ -18364,7 +18364,7 @@
       <c r="AS100" s="86"/>
       <c r="AT100" s="86"/>
     </row>
-    <row r="101" spans="1:49" s="89" customFormat="1">
+    <row r="101" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A101" s="86" t="s">
         <v>14</v>
       </c>
@@ -18405,7 +18405,7 @@
       <c r="AS101" s="86"/>
       <c r="AT101" s="86"/>
     </row>
-    <row r="102" spans="1:49" s="89" customFormat="1" ht="70">
+    <row r="102" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A102" s="86" t="s">
         <v>14</v>
       </c>
@@ -18446,7 +18446,7 @@
       <c r="AS102" s="86"/>
       <c r="AT102" s="86"/>
     </row>
-    <row r="103" spans="1:49" s="89" customFormat="1" ht="42">
+    <row r="103" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A103" s="86" t="s">
         <v>14</v>
       </c>
@@ -18487,7 +18487,7 @@
       <c r="AS103" s="86"/>
       <c r="AT103" s="86"/>
     </row>
-    <row r="104" spans="1:49" s="89" customFormat="1">
+    <row r="104" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A104" s="86" t="s">
         <v>27</v>
       </c>
@@ -18526,7 +18526,7 @@
       <c r="AS104" s="86"/>
       <c r="AT104" s="86"/>
     </row>
-    <row r="105" spans="1:49" s="94" customFormat="1" ht="98">
+    <row r="105" spans="1:49" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A105" s="86" t="s">
         <v>20</v>
       </c>
@@ -18568,7 +18568,7 @@
       <c r="X105" s="75"/>
       <c r="Y105" s="75"/>
     </row>
-    <row r="106" spans="1:49" s="89" customFormat="1" ht="126">
+    <row r="106" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A106" s="86" t="s">
         <v>20</v>
       </c>
@@ -18615,7 +18615,7 @@
       <c r="AS106" s="86"/>
       <c r="AT106" s="86"/>
     </row>
-    <row r="107" spans="1:49" s="89" customFormat="1" ht="126">
+    <row r="107" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A107" s="86" t="s">
         <v>20</v>
       </c>
@@ -18662,7 +18662,7 @@
       <c r="AS107" s="86"/>
       <c r="AT107" s="86"/>
     </row>
-    <row r="108" spans="1:49" s="89" customFormat="1" ht="224">
+    <row r="108" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A108" s="86" t="s">
         <v>20</v>
       </c>
@@ -18709,7 +18709,7 @@
       <c r="AS108" s="86"/>
       <c r="AT108" s="86"/>
     </row>
-    <row r="109" spans="1:49" s="89" customFormat="1" ht="140">
+    <row r="109" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A109" s="86" t="s">
         <v>20</v>
       </c>
@@ -18756,7 +18756,7 @@
       <c r="AS109" s="86"/>
       <c r="AT109" s="86"/>
     </row>
-    <row r="110" spans="1:49" ht="42">
+    <row r="110" spans="1:49" ht="13" customHeight="1">
       <c r="A110" s="73" t="s">
         <v>14</v>
       </c>
@@ -18793,7 +18793,7 @@
       </c>
       <c r="U110" s="75"/>
     </row>
-    <row r="111" spans="1:49" ht="42">
+    <row r="111" spans="1:49" ht="13" customHeight="1">
       <c r="A111" s="73" t="s">
         <v>14</v>
       </c>
@@ -18830,7 +18830,7 @@
       </c>
       <c r="U111" s="75"/>
     </row>
-    <row r="112" spans="1:49" ht="168">
+    <row r="112" spans="1:49" ht="13" customHeight="1">
       <c r="A112" s="73" t="s">
         <v>14</v>
       </c>
@@ -18867,7 +18867,7 @@
       </c>
       <c r="U112" s="75"/>
     </row>
-    <row r="113" spans="1:49" ht="98">
+    <row r="113" spans="1:49" ht="13" customHeight="1">
       <c r="A113" s="73" t="s">
         <v>28</v>
       </c>
@@ -18913,7 +18913,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="114" spans="1:49" s="78" customFormat="1" ht="70">
+    <row r="114" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A114" s="77" t="s">
         <v>162</v>
       </c>
@@ -18959,7 +18959,7 @@
       <c r="X114" s="77"/>
       <c r="Y114" s="77"/>
     </row>
-    <row r="115" spans="1:49" s="85" customFormat="1" ht="98">
+    <row r="115" spans="1:49" s="85" customFormat="1" ht="13" customHeight="1">
       <c r="A115" s="84" t="s">
         <v>20</v>
       </c>
@@ -19009,7 +19009,7 @@
       <c r="X115" s="84"/>
       <c r="Y115" s="84"/>
     </row>
-    <row r="116" spans="1:49" s="78" customFormat="1" ht="70">
+    <row r="116" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A116" s="77" t="s">
         <v>200</v>
       </c>
@@ -19055,7 +19055,7 @@
       <c r="X116" s="77"/>
       <c r="Y116" s="77"/>
     </row>
-    <row r="117" spans="1:49" s="78" customFormat="1" ht="42">
+    <row r="117" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A117" s="77" t="s">
         <v>46</v>
       </c>
@@ -19107,7 +19107,7 @@
       <c r="X117" s="77"/>
       <c r="Y117" s="77"/>
     </row>
-    <row r="118" spans="1:49" s="89" customFormat="1">
+    <row r="118" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A118" s="86" t="s">
         <v>16</v>
       </c>
@@ -19154,7 +19154,7 @@
       <c r="AS118" s="86"/>
       <c r="AT118" s="86"/>
     </row>
-    <row r="119" spans="1:49" s="78" customFormat="1" ht="294">
+    <row r="119" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A119" s="77" t="s">
         <v>20</v>
       </c>
@@ -19216,7 +19216,7 @@
       <c r="AV119" s="77"/>
       <c r="AW119" s="77"/>
     </row>
-    <row r="120" spans="1:49" s="89" customFormat="1" ht="28">
+    <row r="120" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A120" s="86" t="s">
         <v>1665</v>
       </c>
@@ -19261,7 +19261,7 @@
       <c r="AS120" s="86"/>
       <c r="AT120" s="86"/>
     </row>
-    <row r="121" spans="1:49" s="89" customFormat="1" ht="56">
+    <row r="121" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A121" s="86" t="s">
         <v>122</v>
       </c>
@@ -19314,7 +19314,7 @@
       <c r="AS121" s="86"/>
       <c r="AT121" s="86"/>
     </row>
-    <row r="122" spans="1:49" s="89" customFormat="1">
+    <row r="122" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A122" s="86" t="s">
         <v>14</v>
       </c>
@@ -19355,7 +19355,7 @@
       <c r="AS122" s="86"/>
       <c r="AT122" s="86"/>
     </row>
-    <row r="123" spans="1:49" s="89" customFormat="1" ht="70">
+    <row r="123" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A123" s="86" t="s">
         <v>14</v>
       </c>
@@ -19396,7 +19396,7 @@
       <c r="AS123" s="86"/>
       <c r="AT123" s="86"/>
     </row>
-    <row r="124" spans="1:49" s="89" customFormat="1" ht="28">
+    <row r="124" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A124" s="86" t="s">
         <v>14</v>
       </c>
@@ -19437,7 +19437,7 @@
       <c r="AS124" s="86"/>
       <c r="AT124" s="86"/>
     </row>
-    <row r="125" spans="1:49" s="89" customFormat="1">
+    <row r="125" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A125" s="86" t="s">
         <v>27</v>
       </c>
@@ -19476,7 +19476,7 @@
       <c r="AS125" s="86"/>
       <c r="AT125" s="86"/>
     </row>
-    <row r="126" spans="1:49" s="94" customFormat="1" ht="70">
+    <row r="126" spans="1:49" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A126" s="86" t="s">
         <v>20</v>
       </c>
@@ -19518,7 +19518,7 @@
       <c r="X126" s="75"/>
       <c r="Y126" s="75"/>
     </row>
-    <row r="127" spans="1:49" s="94" customFormat="1" ht="84">
+    <row r="127" spans="1:49" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A127" s="86" t="s">
         <v>20</v>
       </c>
@@ -19560,7 +19560,7 @@
       <c r="X127" s="75"/>
       <c r="Y127" s="75"/>
     </row>
-    <row r="128" spans="1:49" s="89" customFormat="1">
+    <row r="128" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A128" s="86" t="s">
         <v>16</v>
       </c>
@@ -19607,7 +19607,7 @@
       <c r="AS128" s="86"/>
       <c r="AT128" s="86"/>
     </row>
-    <row r="129" spans="1:49" s="78" customFormat="1" ht="112">
+    <row r="129" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A129" s="77" t="s">
         <v>20</v>
       </c>
@@ -19669,7 +19669,7 @@
       <c r="AV129" s="77"/>
       <c r="AW129" s="77"/>
     </row>
-    <row r="130" spans="1:49" s="89" customFormat="1" ht="28">
+    <row r="130" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A130" s="86" t="s">
         <v>1665</v>
       </c>
@@ -19714,7 +19714,7 @@
       <c r="AS130" s="86"/>
       <c r="AT130" s="86"/>
     </row>
-    <row r="131" spans="1:49" s="89" customFormat="1" ht="56">
+    <row r="131" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A131" s="86" t="s">
         <v>122</v>
       </c>
@@ -19767,7 +19767,7 @@
       <c r="AS131" s="86"/>
       <c r="AT131" s="86"/>
     </row>
-    <row r="132" spans="1:49" s="89" customFormat="1">
+    <row r="132" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A132" s="86" t="s">
         <v>14</v>
       </c>
@@ -19808,7 +19808,7 @@
       <c r="AS132" s="86"/>
       <c r="AT132" s="86"/>
     </row>
-    <row r="133" spans="1:49" s="89" customFormat="1" ht="70">
+    <row r="133" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A133" s="86" t="s">
         <v>14</v>
       </c>
@@ -19849,7 +19849,7 @@
       <c r="AS133" s="86"/>
       <c r="AT133" s="86"/>
     </row>
-    <row r="134" spans="1:49" s="89" customFormat="1" ht="28">
+    <row r="134" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A134" s="86" t="s">
         <v>14</v>
       </c>
@@ -19890,7 +19890,7 @@
       <c r="AS134" s="86"/>
       <c r="AT134" s="86"/>
     </row>
-    <row r="135" spans="1:49" s="89" customFormat="1">
+    <row r="135" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A135" s="86" t="s">
         <v>27</v>
       </c>
@@ -19929,7 +19929,7 @@
       <c r="AS135" s="86"/>
       <c r="AT135" s="86"/>
     </row>
-    <row r="136" spans="1:49" s="94" customFormat="1" ht="70">
+    <row r="136" spans="1:49" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A136" s="86" t="s">
         <v>20</v>
       </c>
@@ -19971,7 +19971,7 @@
       <c r="X136" s="75"/>
       <c r="Y136" s="75"/>
     </row>
-    <row r="137" spans="1:49" s="94" customFormat="1" ht="98">
+    <row r="137" spans="1:49" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A137" s="86" t="s">
         <v>20</v>
       </c>
@@ -20013,7 +20013,7 @@
       <c r="X137" s="75"/>
       <c r="Y137" s="75"/>
     </row>
-    <row r="138" spans="1:49" s="89" customFormat="1" ht="168">
+    <row r="138" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A138" s="86" t="s">
         <v>20</v>
       </c>
@@ -20060,7 +20060,7 @@
       <c r="AS138" s="86"/>
       <c r="AT138" s="86"/>
     </row>
-    <row r="139" spans="1:49" s="89" customFormat="1" ht="98">
+    <row r="139" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A139" s="86" t="s">
         <v>20</v>
       </c>
@@ -20107,7 +20107,7 @@
       <c r="AS139" s="86"/>
       <c r="AT139" s="86"/>
     </row>
-    <row r="140" spans="1:49" ht="28">
+    <row r="140" spans="1:49" ht="13" customHeight="1">
       <c r="A140" s="73" t="s">
         <v>180</v>
       </c>
@@ -20151,7 +20151,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="141" spans="1:49" ht="42">
+    <row r="141" spans="1:49" ht="13" customHeight="1">
       <c r="A141" s="73" t="s">
         <v>14</v>
       </c>
@@ -20187,7 +20187,7 @@
       </c>
       <c r="U141" s="75"/>
     </row>
-    <row r="142" spans="1:49" ht="28">
+    <row r="142" spans="1:49" ht="13" customHeight="1">
       <c r="A142" s="73" t="s">
         <v>14</v>
       </c>
@@ -20224,7 +20224,7 @@
       </c>
       <c r="U142" s="75"/>
     </row>
-    <row r="143" spans="1:49">
+    <row r="143" spans="1:49" ht="13" customHeight="1">
       <c r="A143" s="73" t="s">
         <v>16</v>
       </c>
@@ -20263,7 +20263,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="144" spans="1:49" ht="28">
+    <row r="144" spans="1:49" ht="13" customHeight="1">
       <c r="A144" s="73" t="s">
         <v>20</v>
       </c>
@@ -20302,7 +20302,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="145" spans="1:70" ht="28">
+    <row r="145" spans="1:70" ht="13" customHeight="1">
       <c r="A145" s="73" t="s">
         <v>20</v>
       </c>
@@ -20342,7 +20342,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="146" spans="1:70" ht="140">
+    <row r="146" spans="1:70" ht="13" customHeight="1">
       <c r="A146" s="73" t="s">
         <v>46</v>
       </c>
@@ -20391,7 +20391,7 @@
         <v>2191</v>
       </c>
     </row>
-    <row r="147" spans="1:70" s="74" customFormat="1">
+    <row r="147" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A147" s="73" t="s">
         <v>27</v>
       </c>
@@ -20473,7 +20473,7 @@
       <c r="BQ147" s="75"/>
       <c r="BR147" s="75"/>
     </row>
-    <row r="148" spans="1:70" ht="182">
+    <row r="148" spans="1:70" ht="13" customHeight="1">
       <c r="A148" s="73" t="s">
         <v>166</v>
       </c>
@@ -20522,7 +20522,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="149" spans="1:70" ht="112">
+    <row r="149" spans="1:70" ht="13" customHeight="1">
       <c r="A149" s="73" t="s">
         <v>14</v>
       </c>
@@ -20556,7 +20556,7 @@
       </c>
       <c r="U149" s="75"/>
     </row>
-    <row r="150" spans="1:70" ht="84">
+    <row r="150" spans="1:70" ht="13" customHeight="1">
       <c r="A150" s="73" t="s">
         <v>28</v>
       </c>
@@ -20610,7 +20610,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="151" spans="1:70" ht="112">
+    <row r="151" spans="1:70" ht="13" customHeight="1">
       <c r="A151" s="73" t="s">
         <v>46</v>
       </c>
@@ -20666,7 +20666,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="152" spans="1:70" ht="294">
+    <row r="152" spans="1:70" ht="13" customHeight="1">
       <c r="A152" s="73" t="s">
         <v>28</v>
       </c>
@@ -20720,7 +20720,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="153" spans="1:70" ht="84">
+    <row r="153" spans="1:70" ht="13" customHeight="1">
       <c r="A153" s="73" t="s">
         <v>28</v>
       </c>
@@ -20774,7 +20774,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="154" spans="1:70" s="74" customFormat="1" ht="28">
+    <row r="154" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A154" s="73" t="s">
         <v>16</v>
       </c>
@@ -20862,7 +20862,7 @@
       <c r="BQ154" s="75"/>
       <c r="BR154" s="75"/>
     </row>
-    <row r="155" spans="1:70" s="74" customFormat="1" ht="98">
+    <row r="155" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A155" s="73" t="s">
         <v>20</v>
       </c>
@@ -20952,7 +20952,7 @@
       <c r="BQ155" s="75"/>
       <c r="BR155" s="75"/>
     </row>
-    <row r="156" spans="1:70" s="74" customFormat="1" ht="42">
+    <row r="156" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A156" s="73" t="s">
         <v>20</v>
       </c>
@@ -21042,7 +21042,7 @@
       <c r="BQ156" s="75"/>
       <c r="BR156" s="75"/>
     </row>
-    <row r="157" spans="1:70" s="74" customFormat="1" ht="70">
+    <row r="157" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A157" s="73" t="s">
         <v>20</v>
       </c>
@@ -21132,7 +21132,7 @@
       <c r="BQ157" s="75"/>
       <c r="BR157" s="75"/>
     </row>
-    <row r="158" spans="1:70" s="74" customFormat="1" ht="70">
+    <row r="158" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A158" s="73" t="s">
         <v>20</v>
       </c>
@@ -21222,7 +21222,7 @@
       <c r="BQ158" s="75"/>
       <c r="BR158" s="75"/>
     </row>
-    <row r="159" spans="1:70" s="74" customFormat="1" ht="42">
+    <row r="159" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A159" s="73" t="s">
         <v>198</v>
       </c>
@@ -21308,7 +21308,7 @@
       <c r="BQ159" s="75"/>
       <c r="BR159" s="75"/>
     </row>
-    <row r="160" spans="1:70" s="74" customFormat="1">
+    <row r="160" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A160" s="73" t="s">
         <v>27</v>
       </c>
@@ -21390,7 +21390,7 @@
       <c r="BQ160" s="75"/>
       <c r="BR160" s="75"/>
     </row>
-    <row r="161" spans="1:70" s="78" customFormat="1" ht="28">
+    <row r="161" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A161" s="77" t="s">
         <v>20</v>
       </c>
@@ -21434,7 +21434,7 @@
       <c r="X161" s="77"/>
       <c r="Y161" s="77"/>
     </row>
-    <row r="162" spans="1:70" s="74" customFormat="1" ht="56">
+    <row r="162" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A162" s="73" t="s">
         <v>781</v>
       </c>
@@ -21526,7 +21526,7 @@
       <c r="BQ162" s="75"/>
       <c r="BR162" s="75"/>
     </row>
-    <row r="163" spans="1:70" s="74" customFormat="1" ht="42">
+    <row r="163" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A163" s="73" t="s">
         <v>784</v>
       </c>
@@ -21618,7 +21618,7 @@
       <c r="BQ163" s="75"/>
       <c r="BR163" s="75"/>
     </row>
-    <row r="164" spans="1:70" s="74" customFormat="1" ht="70">
+    <row r="164" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A164" s="73" t="s">
         <v>784</v>
       </c>
@@ -21710,7 +21710,7 @@
       <c r="BQ164" s="75"/>
       <c r="BR164" s="75"/>
     </row>
-    <row r="165" spans="1:70" s="74" customFormat="1" ht="280">
+    <row r="165" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A165" s="73" t="s">
         <v>193</v>
       </c>
@@ -21806,7 +21806,7 @@
       <c r="BQ165" s="75"/>
       <c r="BR165" s="75"/>
     </row>
-    <row r="166" spans="1:70" s="74" customFormat="1" ht="280">
+    <row r="166" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A166" s="73" t="s">
         <v>193</v>
       </c>
@@ -21904,7 +21904,7 @@
       <c r="BQ166" s="75"/>
       <c r="BR166" s="75"/>
     </row>
-    <row r="167" spans="1:70" s="74" customFormat="1" ht="280">
+    <row r="167" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A167" s="73" t="s">
         <v>193</v>
       </c>
@@ -22000,7 +22000,7 @@
       <c r="BQ167" s="75"/>
       <c r="BR167" s="75"/>
     </row>
-    <row r="168" spans="1:70" s="74" customFormat="1" ht="350">
+    <row r="168" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A168" s="73" t="s">
         <v>14</v>
       </c>
@@ -22084,7 +22084,7 @@
       <c r="BQ168" s="75"/>
       <c r="BR168" s="75"/>
     </row>
-    <row r="169" spans="1:70" s="74" customFormat="1" ht="168">
+    <row r="169" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A169" s="73" t="s">
         <v>46</v>
       </c>
@@ -22182,7 +22182,7 @@
       <c r="BQ169" s="75"/>
       <c r="BR169" s="75"/>
     </row>
-    <row r="170" spans="1:70" s="85" customFormat="1" ht="409">
+    <row r="170" spans="1:70" s="85" customFormat="1" ht="13" customHeight="1">
       <c r="A170" s="84" t="s">
         <v>20</v>
       </c>
@@ -22230,7 +22230,7 @@
       <c r="X170" s="84"/>
       <c r="Y170" s="84"/>
     </row>
-    <row r="171" spans="1:70" ht="84">
+    <row r="171" spans="1:70" ht="13" customHeight="1">
       <c r="A171" s="73" t="s">
         <v>200</v>
       </c>
@@ -22274,7 +22274,7 @@
         <v>2134</v>
       </c>
     </row>
-    <row r="172" spans="1:70" ht="84">
+    <row r="172" spans="1:70" ht="13" customHeight="1">
       <c r="A172" s="73" t="s">
         <v>200</v>
       </c>
@@ -22318,7 +22318,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="173" spans="1:70" ht="126">
+    <row r="173" spans="1:70" ht="13" customHeight="1">
       <c r="A173" s="73" t="s">
         <v>200</v>
       </c>
@@ -22367,7 +22367,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="174" spans="1:70" ht="84">
+    <row r="174" spans="1:70" ht="13" customHeight="1">
       <c r="A174" s="73" t="s">
         <v>200</v>
       </c>
@@ -22416,7 +22416,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="175" spans="1:70" ht="98">
+    <row r="175" spans="1:70" ht="13" customHeight="1">
       <c r="A175" s="73" t="s">
         <v>200</v>
       </c>
@@ -22465,7 +22465,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="176" spans="1:70" ht="84">
+    <row r="176" spans="1:70" ht="13" customHeight="1">
       <c r="A176" s="73" t="s">
         <v>200</v>
       </c>
@@ -22514,7 +22514,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="177" spans="1:25" ht="126">
+    <row r="177" spans="1:25" ht="13" customHeight="1">
       <c r="A177" s="73" t="s">
         <v>200</v>
       </c>
@@ -22558,7 +22558,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="178" spans="1:25" ht="84">
+    <row r="178" spans="1:25" ht="13" customHeight="1">
       <c r="A178" s="73" t="s">
         <v>200</v>
       </c>
@@ -22607,7 +22607,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="179" spans="1:25" ht="84">
+    <row r="179" spans="1:25" ht="13" customHeight="1">
       <c r="A179" s="73" t="s">
         <v>200</v>
       </c>
@@ -22656,7 +22656,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="180" spans="1:25" ht="98">
+    <row r="180" spans="1:25" ht="13" customHeight="1">
       <c r="A180" s="73" t="s">
         <v>200</v>
       </c>
@@ -22705,7 +22705,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="181" spans="1:25" ht="140">
+    <row r="181" spans="1:25" ht="13" customHeight="1">
       <c r="A181" s="73" t="s">
         <v>200</v>
       </c>
@@ -22754,7 +22754,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="182" spans="1:25" ht="140">
+    <row r="182" spans="1:25" ht="13" customHeight="1">
       <c r="A182" s="73" t="s">
         <v>200</v>
       </c>
@@ -22803,7 +22803,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="183" spans="1:25" ht="42">
+    <row r="183" spans="1:25" ht="13" customHeight="1">
       <c r="A183" s="73" t="s">
         <v>200</v>
       </c>
@@ -22847,7 +22847,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="184" spans="1:25" ht="112">
+    <row r="184" spans="1:25" ht="13" customHeight="1">
       <c r="A184" s="73" t="s">
         <v>200</v>
       </c>
@@ -22891,7 +22891,7 @@
         <v>2139</v>
       </c>
     </row>
-    <row r="185" spans="1:25" ht="98">
+    <row r="185" spans="1:25" ht="13" customHeight="1">
       <c r="A185" s="73" t="s">
         <v>200</v>
       </c>
@@ -22935,7 +22935,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="186" spans="1:25" ht="56">
+    <row r="186" spans="1:25" ht="13" customHeight="1">
       <c r="A186" s="73" t="s">
         <v>200</v>
       </c>
@@ -22979,7 +22979,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="187" spans="1:25" ht="140">
+    <row r="187" spans="1:25" ht="13" customHeight="1">
       <c r="A187" s="73" t="s">
         <v>200</v>
       </c>
@@ -23023,7 +23023,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="188" spans="1:25" s="78" customFormat="1">
+    <row r="188" spans="1:25" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A188" s="77" t="s">
         <v>16</v>
       </c>
@@ -23065,7 +23065,7 @@
       <c r="X188" s="77"/>
       <c r="Y188" s="77"/>
     </row>
-    <row r="189" spans="1:25" s="78" customFormat="1" ht="112">
+    <row r="189" spans="1:25" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A189" s="77" t="s">
         <v>225</v>
       </c>
@@ -23119,7 +23119,7 @@
       </c>
       <c r="Y189" s="77"/>
     </row>
-    <row r="190" spans="1:25" s="78" customFormat="1" ht="28">
+    <row r="190" spans="1:25" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A190" s="77" t="s">
         <v>104</v>
       </c>
@@ -23159,7 +23159,7 @@
       <c r="X190" s="77"/>
       <c r="Y190" s="77"/>
     </row>
-    <row r="191" spans="1:25" s="78" customFormat="1">
+    <row r="191" spans="1:25" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A191" s="77" t="s">
         <v>27</v>
       </c>
@@ -23193,7 +23193,7 @@
       <c r="X191" s="77"/>
       <c r="Y191" s="77"/>
     </row>
-    <row r="192" spans="1:25" s="78" customFormat="1" ht="56">
+    <row r="192" spans="1:25" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A192" s="77" t="s">
         <v>14</v>
       </c>
@@ -23237,7 +23237,7 @@
       <c r="X192" s="77"/>
       <c r="Y192" s="77"/>
     </row>
-    <row r="193" spans="1:70" s="180" customFormat="1" ht="196">
+    <row r="193" spans="1:70" s="180" customFormat="1" ht="13" customHeight="1">
       <c r="A193" s="178" t="s">
         <v>291</v>
       </c>
@@ -23285,7 +23285,7 @@
       <c r="X193" s="178"/>
       <c r="Y193" s="178"/>
     </row>
-    <row r="194" spans="1:70" s="78" customFormat="1" ht="42">
+    <row r="194" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A194" s="77" t="s">
         <v>1030</v>
       </c>
@@ -23339,7 +23339,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="195" spans="1:70" s="78" customFormat="1" ht="56">
+    <row r="195" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A195" s="77" t="s">
         <v>200</v>
       </c>
@@ -23385,7 +23385,7 @@
       <c r="X195" s="77"/>
       <c r="Y195" s="77"/>
     </row>
-    <row r="196" spans="1:70" s="78" customFormat="1" ht="42">
+    <row r="196" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A196" s="77" t="s">
         <v>200</v>
       </c>
@@ -23430,7 +23430,7 @@
       <c r="X196" s="77"/>
       <c r="Y196" s="77"/>
     </row>
-    <row r="197" spans="1:70" s="138" customFormat="1" ht="168">
+    <row r="197" spans="1:70" s="138" customFormat="1" ht="13" customHeight="1">
       <c r="A197" s="133" t="s">
         <v>28</v>
       </c>
@@ -23528,7 +23528,7 @@
       <c r="BQ197" s="137"/>
       <c r="BR197" s="137"/>
     </row>
-    <row r="198" spans="1:70" s="138" customFormat="1" ht="28">
+    <row r="198" spans="1:70" s="138" customFormat="1" ht="13" customHeight="1">
       <c r="A198" s="139" t="s">
         <v>1013</v>
       </c>
@@ -23620,7 +23620,7 @@
       <c r="BQ198" s="137"/>
       <c r="BR198" s="137"/>
     </row>
-    <row r="199" spans="1:70" s="138" customFormat="1" ht="70">
+    <row r="199" spans="1:70" s="138" customFormat="1" ht="13" customHeight="1">
       <c r="A199" s="141" t="s">
         <v>200</v>
       </c>
@@ -23712,7 +23712,7 @@
       <c r="BQ199" s="137"/>
       <c r="BR199" s="137"/>
     </row>
-    <row r="200" spans="1:70" s="138" customFormat="1" ht="210">
+    <row r="200" spans="1:70" s="138" customFormat="1" ht="13" customHeight="1">
       <c r="A200" s="141" t="s">
         <v>1017</v>
       </c>
@@ -23808,7 +23808,7 @@
       <c r="BQ200" s="137"/>
       <c r="BR200" s="137"/>
     </row>
-    <row r="201" spans="1:70" s="137" customFormat="1" ht="70">
+    <row r="201" spans="1:70" s="137" customFormat="1" ht="13" customHeight="1">
       <c r="A201" s="141" t="s">
         <v>14</v>
       </c>
@@ -23844,7 +23844,7 @@
       <c r="X201" s="136"/>
       <c r="Y201" s="136"/>
     </row>
-    <row r="202" spans="1:70" s="148" customFormat="1" ht="56">
+    <row r="202" spans="1:70" s="148" customFormat="1" ht="13" customHeight="1">
       <c r="A202" s="144" t="s">
         <v>46</v>
       </c>
@@ -23942,7 +23942,7 @@
       <c r="BQ202" s="147"/>
       <c r="BR202" s="147"/>
     </row>
-    <row r="203" spans="1:70" s="78" customFormat="1" ht="84">
+    <row r="203" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A203" s="77" t="s">
         <v>200</v>
       </c>
@@ -23988,7 +23988,7 @@
       <c r="X203" s="77"/>
       <c r="Y203" s="77"/>
     </row>
-    <row r="204" spans="1:70" ht="84">
+    <row r="204" spans="1:70" ht="13" customHeight="1">
       <c r="A204" s="73" t="s">
         <v>200</v>
       </c>
@@ -24032,7 +24032,7 @@
         <v>2144</v>
       </c>
     </row>
-    <row r="205" spans="1:70" ht="56">
+    <row r="205" spans="1:70" ht="13" customHeight="1">
       <c r="A205" s="73" t="s">
         <v>200</v>
       </c>
@@ -24076,7 +24076,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="206" spans="1:70" ht="56">
+    <row r="206" spans="1:70" ht="13" customHeight="1">
       <c r="A206" s="73" t="s">
         <v>200</v>
       </c>
@@ -24120,7 +24120,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="207" spans="1:70" s="78" customFormat="1">
+    <row r="207" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A207" s="77" t="s">
         <v>16</v>
       </c>
@@ -24162,7 +24162,7 @@
       <c r="X207" s="77"/>
       <c r="Y207" s="77"/>
     </row>
-    <row r="208" spans="1:70" s="78" customFormat="1" ht="126">
+    <row r="208" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A208" s="77" t="s">
         <v>241</v>
       </c>
@@ -24210,7 +24210,7 @@
       <c r="X208" s="77"/>
       <c r="Y208" s="77"/>
     </row>
-    <row r="209" spans="1:70" s="78" customFormat="1" ht="28">
+    <row r="209" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A209" s="77" t="s">
         <v>104</v>
       </c>
@@ -24250,7 +24250,7 @@
       <c r="X209" s="77"/>
       <c r="Y209" s="77"/>
     </row>
-    <row r="210" spans="1:70" s="78" customFormat="1">
+    <row r="210" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A210" s="77" t="s">
         <v>27</v>
       </c>
@@ -24284,7 +24284,7 @@
       <c r="X210" s="77"/>
       <c r="Y210" s="77"/>
     </row>
-    <row r="211" spans="1:70" s="78" customFormat="1" ht="42">
+    <row r="211" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A211" s="77" t="s">
         <v>1030</v>
       </c>
@@ -24338,7 +24338,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="212" spans="1:70" ht="28">
+    <row r="212" spans="1:70" ht="13" customHeight="1">
       <c r="A212" s="73" t="s">
         <v>14</v>
       </c>
@@ -24374,7 +24374,7 @@
       <c r="X212" s="77"/>
       <c r="Y212" s="77"/>
     </row>
-    <row r="213" spans="1:70" ht="56">
+    <row r="213" spans="1:70" ht="13" customHeight="1">
       <c r="A213" s="73" t="s">
         <v>14</v>
       </c>
@@ -24410,7 +24410,7 @@
       <c r="X213" s="77"/>
       <c r="Y213" s="77"/>
     </row>
-    <row r="214" spans="1:70" ht="70">
+    <row r="214" spans="1:70" ht="13" customHeight="1">
       <c r="A214" s="73" t="s">
         <v>14</v>
       </c>
@@ -24446,7 +24446,7 @@
       <c r="X214" s="77"/>
       <c r="Y214" s="77"/>
     </row>
-    <row r="215" spans="1:70" ht="112">
+    <row r="215" spans="1:70" ht="13" customHeight="1">
       <c r="A215" s="73" t="s">
         <v>14</v>
       </c>
@@ -24482,7 +24482,7 @@
       <c r="X215" s="77"/>
       <c r="Y215" s="77"/>
     </row>
-    <row r="216" spans="1:70" ht="84">
+    <row r="216" spans="1:70" ht="13" customHeight="1">
       <c r="A216" s="73" t="s">
         <v>162</v>
       </c>
@@ -24528,7 +24528,7 @@
       <c r="X216" s="77"/>
       <c r="Y216" s="77"/>
     </row>
-    <row r="217" spans="1:70" ht="70">
+    <row r="217" spans="1:70" ht="13" customHeight="1">
       <c r="A217" s="73" t="s">
         <v>825</v>
       </c>
@@ -24574,7 +24574,7 @@
       <c r="X217" s="77"/>
       <c r="Y217" s="77"/>
     </row>
-    <row r="218" spans="1:70" s="99" customFormat="1" ht="42">
+    <row r="218" spans="1:70" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A218" s="77" t="s">
         <v>14</v>
       </c>
@@ -24656,7 +24656,7 @@
       <c r="BQ218" s="77"/>
       <c r="BR218" s="77"/>
     </row>
-    <row r="219" spans="1:70" s="103" customFormat="1" ht="168">
+    <row r="219" spans="1:70" s="103" customFormat="1" ht="13" customHeight="1">
       <c r="A219" s="77" t="s">
         <v>46</v>
       </c>
@@ -24754,7 +24754,7 @@
       <c r="BQ219" s="101"/>
       <c r="BR219" s="101"/>
     </row>
-    <row r="220" spans="1:70" s="86" customFormat="1">
+    <row r="220" spans="1:70" s="86" customFormat="1" ht="13" customHeight="1">
       <c r="A220" s="86" t="s">
         <v>16</v>
       </c>
@@ -24784,7 +24784,7 @@
       <c r="X220" s="75"/>
       <c r="Y220" s="75"/>
     </row>
-    <row r="221" spans="1:70" s="78" customFormat="1" ht="84">
+    <row r="221" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A221" s="77" t="s">
         <v>20</v>
       </c>
@@ -24854,7 +24854,7 @@
       <c r="AV221" s="77"/>
       <c r="AW221" s="77"/>
     </row>
-    <row r="222" spans="1:70" s="78" customFormat="1" ht="28">
+    <row r="222" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A222" s="77" t="s">
         <v>20</v>
       </c>
@@ -24914,7 +24914,7 @@
       <c r="AV222" s="77"/>
       <c r="AW222" s="77"/>
     </row>
-    <row r="223" spans="1:70" s="78" customFormat="1" ht="28">
+    <row r="223" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A223" s="77" t="s">
         <v>20</v>
       </c>
@@ -24974,7 +24974,7 @@
       <c r="AV223" s="77"/>
       <c r="AW223" s="77"/>
     </row>
-    <row r="224" spans="1:70" s="89" customFormat="1" ht="28">
+    <row r="224" spans="1:70" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A224" s="86" t="s">
         <v>1665</v>
       </c>
@@ -25019,7 +25019,7 @@
       <c r="AS224" s="86"/>
       <c r="AT224" s="86"/>
     </row>
-    <row r="225" spans="1:49" s="89" customFormat="1" ht="56">
+    <row r="225" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A225" s="86" t="s">
         <v>122</v>
       </c>
@@ -25072,7 +25072,7 @@
       <c r="AS225" s="86"/>
       <c r="AT225" s="86"/>
     </row>
-    <row r="226" spans="1:49" s="89" customFormat="1">
+    <row r="226" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A226" s="86" t="s">
         <v>14</v>
       </c>
@@ -25113,7 +25113,7 @@
       <c r="AS226" s="86"/>
       <c r="AT226" s="86"/>
     </row>
-    <row r="227" spans="1:49" s="89" customFormat="1" ht="70">
+    <row r="227" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A227" s="86" t="s">
         <v>14</v>
       </c>
@@ -25154,7 +25154,7 @@
       <c r="AS227" s="86"/>
       <c r="AT227" s="86"/>
     </row>
-    <row r="228" spans="1:49" s="89" customFormat="1" ht="28">
+    <row r="228" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A228" s="86" t="s">
         <v>14</v>
       </c>
@@ -25195,7 +25195,7 @@
       <c r="AS228" s="86"/>
       <c r="AT228" s="86"/>
     </row>
-    <row r="229" spans="1:49" s="86" customFormat="1">
+    <row r="229" spans="1:49" s="86" customFormat="1" ht="13" customHeight="1">
       <c r="A229" s="86" t="s">
         <v>27</v>
       </c>
@@ -25217,7 +25217,7 @@
       <c r="X229" s="75"/>
       <c r="Y229" s="75"/>
     </row>
-    <row r="230" spans="1:49" s="94" customFormat="1" ht="70">
+    <row r="230" spans="1:49" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A230" s="86" t="s">
         <v>20</v>
       </c>
@@ -25259,7 +25259,7 @@
       <c r="X230" s="75"/>
       <c r="Y230" s="75"/>
     </row>
-    <row r="231" spans="1:49" s="94" customFormat="1" ht="112">
+    <row r="231" spans="1:49" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A231" s="86" t="s">
         <v>20</v>
       </c>
@@ -25319,7 +25319,7 @@
       <c r="AP231" s="75"/>
       <c r="AQ231" s="75"/>
     </row>
-    <row r="232" spans="1:49" s="86" customFormat="1" ht="154">
+    <row r="232" spans="1:49" s="86" customFormat="1" ht="13" customHeight="1">
       <c r="A232" s="86" t="s">
         <v>20</v>
       </c>
@@ -25369,7 +25369,7 @@
       <c r="AP232" s="75"/>
       <c r="AQ232" s="75"/>
     </row>
-    <row r="233" spans="1:49" s="86" customFormat="1" ht="98">
+    <row r="233" spans="1:49" s="86" customFormat="1" ht="13" customHeight="1">
       <c r="A233" s="86" t="s">
         <v>20</v>
       </c>
@@ -25419,7 +25419,7 @@
       <c r="AP233" s="75"/>
       <c r="AQ233" s="75"/>
     </row>
-    <row r="234" spans="1:49" s="89" customFormat="1">
+    <row r="234" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A234" s="86" t="s">
         <v>16</v>
       </c>
@@ -25482,7 +25482,7 @@
       <c r="AS234" s="86"/>
       <c r="AT234" s="86"/>
     </row>
-    <row r="235" spans="1:49" s="78" customFormat="1" ht="280">
+    <row r="235" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A235" s="77" t="s">
         <v>20</v>
       </c>
@@ -25552,7 +25552,7 @@
       <c r="AV235" s="77"/>
       <c r="AW235" s="77"/>
     </row>
-    <row r="236" spans="1:49" s="89" customFormat="1" ht="28">
+    <row r="236" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A236" s="86" t="s">
         <v>1665</v>
       </c>
@@ -25597,7 +25597,7 @@
       <c r="AS236" s="86"/>
       <c r="AT236" s="86"/>
     </row>
-    <row r="237" spans="1:49" s="89" customFormat="1" ht="56">
+    <row r="237" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A237" s="86" t="s">
         <v>122</v>
       </c>
@@ -25650,7 +25650,7 @@
       <c r="AS237" s="86"/>
       <c r="AT237" s="86"/>
     </row>
-    <row r="238" spans="1:49" s="89" customFormat="1">
+    <row r="238" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A238" s="86" t="s">
         <v>14</v>
       </c>
@@ -25691,7 +25691,7 @@
       <c r="AS238" s="86"/>
       <c r="AT238" s="86"/>
     </row>
-    <row r="239" spans="1:49" s="89" customFormat="1" ht="70">
+    <row r="239" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A239" s="86" t="s">
         <v>14</v>
       </c>
@@ -25732,7 +25732,7 @@
       <c r="AS239" s="86"/>
       <c r="AT239" s="86"/>
     </row>
-    <row r="240" spans="1:49" s="89" customFormat="1" ht="28">
+    <row r="240" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A240" s="86" t="s">
         <v>14</v>
       </c>
@@ -25773,7 +25773,7 @@
       <c r="AS240" s="86"/>
       <c r="AT240" s="86"/>
     </row>
-    <row r="241" spans="1:49" s="89" customFormat="1">
+    <row r="241" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A241" s="86" t="s">
         <v>27</v>
       </c>
@@ -25812,7 +25812,7 @@
       <c r="AS241" s="86"/>
       <c r="AT241" s="86"/>
     </row>
-    <row r="242" spans="1:49" s="94" customFormat="1" ht="70">
+    <row r="242" spans="1:49" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A242" s="86" t="s">
         <v>20</v>
       </c>
@@ -25854,7 +25854,7 @@
       <c r="X242" s="75"/>
       <c r="Y242" s="75"/>
     </row>
-    <row r="243" spans="1:49" s="89" customFormat="1" ht="112">
+    <row r="243" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A243" s="86" t="s">
         <v>20</v>
       </c>
@@ -25901,7 +25901,7 @@
       <c r="AS243" s="86"/>
       <c r="AT243" s="86"/>
     </row>
-    <row r="244" spans="1:49" s="89" customFormat="1" ht="112">
+    <row r="244" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A244" s="86" t="s">
         <v>20</v>
       </c>
@@ -25948,7 +25948,7 @@
       <c r="AS244" s="86"/>
       <c r="AT244" s="86"/>
     </row>
-    <row r="245" spans="1:49" s="86" customFormat="1">
+    <row r="245" spans="1:49" s="86" customFormat="1" ht="13" customHeight="1">
       <c r="A245" s="86" t="s">
         <v>16</v>
       </c>
@@ -25978,7 +25978,7 @@
       <c r="X245" s="75"/>
       <c r="Y245" s="75"/>
     </row>
-    <row r="246" spans="1:49" s="78" customFormat="1" ht="196">
+    <row r="246" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A246" s="77" t="s">
         <v>20</v>
       </c>
@@ -26048,7 +26048,7 @@
       <c r="AV246" s="77"/>
       <c r="AW246" s="77"/>
     </row>
-    <row r="247" spans="1:49" s="78" customFormat="1" ht="28">
+    <row r="247" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A247" s="77" t="s">
         <v>20</v>
       </c>
@@ -26108,7 +26108,7 @@
       <c r="AV247" s="77"/>
       <c r="AW247" s="77"/>
     </row>
-    <row r="248" spans="1:49" s="78" customFormat="1" ht="28">
+    <row r="248" spans="1:49" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A248" s="77" t="s">
         <v>20</v>
       </c>
@@ -26168,7 +26168,7 @@
       <c r="AV248" s="77"/>
       <c r="AW248" s="77"/>
     </row>
-    <row r="249" spans="1:49" s="89" customFormat="1" ht="28">
+    <row r="249" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A249" s="86" t="s">
         <v>1665</v>
       </c>
@@ -26213,7 +26213,7 @@
       <c r="AS249" s="86"/>
       <c r="AT249" s="86"/>
     </row>
-    <row r="250" spans="1:49" s="89" customFormat="1" ht="56">
+    <row r="250" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A250" s="86" t="s">
         <v>122</v>
       </c>
@@ -26266,7 +26266,7 @@
       <c r="AS250" s="86"/>
       <c r="AT250" s="86"/>
     </row>
-    <row r="251" spans="1:49" s="89" customFormat="1">
+    <row r="251" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A251" s="86" t="s">
         <v>14</v>
       </c>
@@ -26307,7 +26307,7 @@
       <c r="AS251" s="86"/>
       <c r="AT251" s="86"/>
     </row>
-    <row r="252" spans="1:49" s="89" customFormat="1" ht="70">
+    <row r="252" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A252" s="86" t="s">
         <v>14</v>
       </c>
@@ -26348,7 +26348,7 @@
       <c r="AS252" s="86"/>
       <c r="AT252" s="86"/>
     </row>
-    <row r="253" spans="1:49" s="89" customFormat="1" ht="42">
+    <row r="253" spans="1:49" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A253" s="86" t="s">
         <v>14</v>
       </c>
@@ -26389,7 +26389,7 @@
       <c r="AS253" s="86"/>
       <c r="AT253" s="86"/>
     </row>
-    <row r="254" spans="1:49" s="86" customFormat="1">
+    <row r="254" spans="1:49" s="86" customFormat="1" ht="13" customHeight="1">
       <c r="A254" s="86" t="s">
         <v>27</v>
       </c>
@@ -26411,7 +26411,7 @@
       <c r="X254" s="75"/>
       <c r="Y254" s="75"/>
     </row>
-    <row r="255" spans="1:49" s="94" customFormat="1" ht="84">
+    <row r="255" spans="1:49" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A255" s="86" t="s">
         <v>20</v>
       </c>
@@ -26453,7 +26453,7 @@
       <c r="X255" s="75"/>
       <c r="Y255" s="75"/>
     </row>
-    <row r="256" spans="1:49" s="94" customFormat="1" ht="409">
+    <row r="256" spans="1:49" s="94" customFormat="1" ht="13" customHeight="1">
       <c r="A256" s="86" t="s">
         <v>20</v>
       </c>
@@ -26495,7 +26495,7 @@
       <c r="X256" s="75"/>
       <c r="Y256" s="75"/>
     </row>
-    <row r="257" spans="1:70" s="89" customFormat="1" ht="126">
+    <row r="257" spans="1:70" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A257" s="86" t="s">
         <v>20</v>
       </c>
@@ -26542,7 +26542,7 @@
       <c r="AS257" s="86"/>
       <c r="AT257" s="86"/>
     </row>
-    <row r="258" spans="1:70" s="89" customFormat="1" ht="112">
+    <row r="258" spans="1:70" s="89" customFormat="1" ht="13" customHeight="1">
       <c r="A258" s="86" t="s">
         <v>20</v>
       </c>
@@ -26589,7 +26589,7 @@
       <c r="AS258" s="86"/>
       <c r="AT258" s="86"/>
     </row>
-    <row r="259" spans="1:70" s="74" customFormat="1" ht="112">
+    <row r="259" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A259" s="73" t="s">
         <v>28</v>
       </c>
@@ -26681,7 +26681,7 @@
       <c r="BQ259" s="75"/>
       <c r="BR259" s="75"/>
     </row>
-    <row r="260" spans="1:70" s="74" customFormat="1" ht="168">
+    <row r="260" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A260" s="73" t="s">
         <v>20</v>
       </c>
@@ -26777,7 +26777,7 @@
       <c r="BQ260" s="75"/>
       <c r="BR260" s="75"/>
     </row>
-    <row r="261" spans="1:70" ht="42">
+    <row r="261" spans="1:70" ht="13" customHeight="1">
       <c r="A261" s="73" t="s">
         <v>1581</v>
       </c>
@@ -26828,7 +26828,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="262" spans="1:70" s="78" customFormat="1" ht="210">
+    <row r="262" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A262" s="77" t="s">
         <v>16</v>
       </c>
@@ -26870,7 +26870,7 @@
       <c r="X262" s="77"/>
       <c r="Y262" s="77"/>
     </row>
-    <row r="263" spans="1:70" s="78" customFormat="1" ht="28">
+    <row r="263" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A263" s="77" t="s">
         <v>14</v>
       </c>
@@ -26906,7 +26906,7 @@
       <c r="X263" s="77"/>
       <c r="Y263" s="77"/>
     </row>
-    <row r="264" spans="1:70" s="90" customFormat="1" ht="42">
+    <row r="264" spans="1:70" s="90" customFormat="1" ht="13" customHeight="1">
       <c r="A264" s="77" t="s">
         <v>14</v>
       </c>
@@ -26990,7 +26990,7 @@
       <c r="BQ264" s="78"/>
       <c r="BR264" s="78"/>
     </row>
-    <row r="265" spans="1:70" s="90" customFormat="1" ht="28">
+    <row r="265" spans="1:70" s="90" customFormat="1" ht="13" customHeight="1">
       <c r="A265" s="77" t="s">
         <v>14</v>
       </c>
@@ -27074,7 +27074,7 @@
       <c r="BQ265" s="78"/>
       <c r="BR265" s="78"/>
     </row>
-    <row r="266" spans="1:70" s="78" customFormat="1" ht="112">
+    <row r="266" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A266" s="77" t="s">
         <v>259</v>
       </c>
@@ -27122,7 +27122,7 @@
       <c r="X266" s="77"/>
       <c r="Y266" s="77"/>
     </row>
-    <row r="267" spans="1:70" s="78" customFormat="1" ht="28">
+    <row r="267" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A267" s="77" t="s">
         <v>104</v>
       </c>
@@ -27162,7 +27162,7 @@
       <c r="X267" s="77"/>
       <c r="Y267" s="77"/>
     </row>
-    <row r="268" spans="1:70" s="78" customFormat="1">
+    <row r="268" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A268" s="77" t="s">
         <v>27</v>
       </c>
@@ -27196,7 +27196,7 @@
       <c r="X268" s="77"/>
       <c r="Y268" s="77"/>
     </row>
-    <row r="269" spans="1:70" ht="112">
+    <row r="269" spans="1:70" ht="13" customHeight="1">
       <c r="A269" s="73" t="s">
         <v>200</v>
       </c>
@@ -27240,7 +27240,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="270" spans="1:70" ht="42">
+    <row r="270" spans="1:70" ht="13" customHeight="1">
       <c r="A270" s="73" t="s">
         <v>200</v>
       </c>
@@ -27284,7 +27284,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="271" spans="1:70" s="96" customFormat="1" ht="70">
+    <row r="271" spans="1:70" s="96" customFormat="1" ht="13" customHeight="1">
       <c r="A271" s="98" t="s">
         <v>162</v>
       </c>
@@ -27376,7 +27376,7 @@
       <c r="BQ271" s="97"/>
       <c r="BR271" s="97"/>
     </row>
-    <row r="272" spans="1:70" ht="98">
+    <row r="272" spans="1:70" ht="13" customHeight="1">
       <c r="A272" s="73" t="s">
         <v>200</v>
       </c>
@@ -27420,7 +27420,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="273" spans="1:70" ht="42">
+    <row r="273" spans="1:70" ht="13" customHeight="1">
       <c r="A273" s="73" t="s">
         <v>200</v>
       </c>
@@ -27464,7 +27464,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="274" spans="1:70" ht="28">
+    <row r="274" spans="1:70" ht="13" customHeight="1">
       <c r="A274" s="73" t="s">
         <v>268</v>
       </c>
@@ -27508,7 +27508,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="275" spans="1:70" ht="42">
+    <row r="275" spans="1:70" ht="13" customHeight="1">
       <c r="A275" s="73" t="s">
         <v>271</v>
       </c>
@@ -27552,7 +27552,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="276" spans="1:70" ht="28">
+    <row r="276" spans="1:70" ht="13" customHeight="1">
       <c r="A276" s="73" t="s">
         <v>271</v>
       </c>
@@ -27598,7 +27598,7 @@
       <c r="X276" s="77"/>
       <c r="Y276" s="77"/>
     </row>
-    <row r="277" spans="1:70" ht="28">
+    <row r="277" spans="1:70" ht="13" customHeight="1">
       <c r="A277" s="73" t="s">
         <v>271</v>
       </c>
@@ -27644,7 +27644,7 @@
       <c r="X277" s="77"/>
       <c r="Y277" s="77"/>
     </row>
-    <row r="278" spans="1:70" ht="98">
+    <row r="278" spans="1:70" ht="13" customHeight="1">
       <c r="A278" s="73" t="s">
         <v>14</v>
       </c>
@@ -27680,7 +27680,7 @@
       <c r="X278" s="77"/>
       <c r="Y278" s="77"/>
     </row>
-    <row r="279" spans="1:70" ht="112">
+    <row r="279" spans="1:70" ht="13" customHeight="1">
       <c r="A279" s="73" t="s">
         <v>162</v>
       </c>
@@ -27724,7 +27724,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="280" spans="1:70" ht="112">
+    <row r="280" spans="1:70" ht="13" customHeight="1">
       <c r="A280" s="73" t="s">
         <v>162</v>
       </c>
@@ -27769,7 +27769,7 @@
       </c>
       <c r="W280"/>
     </row>
-    <row r="281" spans="1:70" s="78" customFormat="1" ht="70">
+    <row r="281" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A281" s="77" t="s">
         <v>1549</v>
       </c>
@@ -27819,7 +27819,7 @@
       <c r="X281" s="77"/>
       <c r="Y281" s="77"/>
     </row>
-    <row r="282" spans="1:70" s="138" customFormat="1" ht="42">
+    <row r="282" spans="1:70" s="138" customFormat="1" ht="13" customHeight="1">
       <c r="A282" s="136" t="s">
         <v>200</v>
       </c>
@@ -27911,7 +27911,7 @@
       <c r="BQ282" s="137"/>
       <c r="BR282" s="137"/>
     </row>
-    <row r="283" spans="1:70" s="138" customFormat="1" ht="42">
+    <row r="283" spans="1:70" s="138" customFormat="1" ht="13" customHeight="1">
       <c r="A283" s="77" t="s">
         <v>1549</v>
       </c>
@@ -28003,7 +28003,7 @@
       <c r="BQ283" s="137"/>
       <c r="BR283" s="137"/>
     </row>
-    <row r="284" spans="1:70" s="138" customFormat="1" ht="42">
+    <row r="284" spans="1:70" s="138" customFormat="1" ht="13" customHeight="1">
       <c r="A284" s="136" t="s">
         <v>1552</v>
       </c>
@@ -28101,7 +28101,7 @@
       <c r="BQ284" s="137"/>
       <c r="BR284" s="137"/>
     </row>
-    <row r="285" spans="1:70" s="138" customFormat="1" ht="28">
+    <row r="285" spans="1:70" s="138" customFormat="1" ht="13" customHeight="1">
       <c r="A285" s="136" t="s">
         <v>37</v>
       </c>
@@ -28195,7 +28195,7 @@
       <c r="BQ285" s="137"/>
       <c r="BR285" s="137"/>
     </row>
-    <row r="286" spans="1:70" s="78" customFormat="1" ht="98">
+    <row r="286" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A286" s="73" t="s">
         <v>200</v>
       </c>
@@ -28241,7 +28241,7 @@
       <c r="X286" s="77"/>
       <c r="Y286" s="77"/>
     </row>
-    <row r="287" spans="1:70" s="78" customFormat="1" ht="42">
+    <row r="287" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A287" s="77" t="s">
         <v>241</v>
       </c>
@@ -28287,7 +28287,7 @@
       <c r="X287" s="77"/>
       <c r="Y287" s="77"/>
     </row>
-    <row r="288" spans="1:70" s="77" customFormat="1" ht="98">
+    <row r="288" spans="1:70" s="77" customFormat="1" ht="13" customHeight="1">
       <c r="A288" s="77" t="s">
         <v>200</v>
       </c>
@@ -28319,7 +28319,7 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="289" spans="1:70" s="77" customFormat="1" ht="126">
+    <row r="289" spans="1:70" s="77" customFormat="1" ht="13" customHeight="1">
       <c r="A289" s="77" t="s">
         <v>2664</v>
       </c>
@@ -28359,7 +28359,7 @@
         <v>2515</v>
       </c>
     </row>
-    <row r="290" spans="1:70" s="99" customFormat="1" ht="112">
+    <row r="290" spans="1:70" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A290" s="77" t="s">
         <v>14</v>
       </c>
@@ -28445,7 +28445,7 @@
       <c r="BQ290" s="77"/>
       <c r="BR290" s="77"/>
     </row>
-    <row r="291" spans="1:70" s="99" customFormat="1" ht="112">
+    <row r="291" spans="1:70" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A291" s="77" t="s">
         <v>46</v>
       </c>
@@ -28547,7 +28547,7 @@
       <c r="BQ291" s="77"/>
       <c r="BR291" s="77"/>
     </row>
-    <row r="292" spans="1:70" s="99" customFormat="1" ht="308">
+    <row r="292" spans="1:70" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A292" s="77" t="s">
         <v>20</v>
       </c>
@@ -28637,7 +28637,7 @@
       <c r="BQ292" s="77"/>
       <c r="BR292" s="77"/>
     </row>
-    <row r="293" spans="1:70" s="77" customFormat="1" ht="112">
+    <row r="293" spans="1:70" s="77" customFormat="1" ht="13" customHeight="1">
       <c r="A293" s="77" t="s">
         <v>291</v>
       </c>
@@ -28669,7 +28669,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="294" spans="1:70" s="77" customFormat="1" ht="70">
+    <row r="294" spans="1:70" s="77" customFormat="1" ht="13" customHeight="1">
       <c r="A294" s="104" t="s">
         <v>20</v>
       </c>
@@ -28730,7 +28730,7 @@
       <c r="AN294" s="104"/>
       <c r="AO294" s="104"/>
     </row>
-    <row r="295" spans="1:70" s="77" customFormat="1" ht="42">
+    <row r="295" spans="1:70" s="77" customFormat="1" ht="13" customHeight="1">
       <c r="A295" s="77" t="s">
         <v>1030</v>
       </c>
@@ -28774,7 +28774,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="296" spans="1:70" s="78" customFormat="1">
+    <row r="296" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A296" s="77"/>
       <c r="B296" s="77"/>
       <c r="C296" s="77"/>
@@ -28802,7 +28802,7 @@
       <c r="X296" s="77"/>
       <c r="Y296" s="77"/>
     </row>
-    <row r="297" spans="1:70" ht="56">
+    <row r="297" spans="1:70" ht="13" customHeight="1">
       <c r="A297" s="73" t="s">
         <v>200</v>
       </c>
@@ -28846,7 +28846,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="298" spans="1:70" s="78" customFormat="1" ht="42">
+    <row r="298" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A298" s="77" t="s">
         <v>14</v>
       </c>
@@ -28882,7 +28882,7 @@
       <c r="X298" s="77"/>
       <c r="Y298" s="77"/>
     </row>
-    <row r="299" spans="1:70" s="184" customFormat="1" ht="210">
+    <row r="299" spans="1:70" s="184" customFormat="1" ht="13" customHeight="1">
       <c r="A299" s="183" t="s">
         <v>14</v>
       </c>
@@ -28912,7 +28912,7 @@
       <c r="X299" s="183"/>
       <c r="Y299" s="183"/>
     </row>
-    <row r="300" spans="1:70" s="78" customFormat="1" ht="210">
+    <row r="300" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A300" s="77" t="s">
         <v>14</v>
       </c>
@@ -28948,7 +28948,7 @@
       <c r="X300" s="77"/>
       <c r="Y300" s="77"/>
     </row>
-    <row r="301" spans="1:70" s="184" customFormat="1" ht="28">
+    <row r="301" spans="1:70" s="184" customFormat="1" ht="13" customHeight="1">
       <c r="A301" s="183" t="s">
         <v>14</v>
       </c>
@@ -28978,7 +28978,7 @@
       <c r="X301" s="183"/>
       <c r="Y301" s="183"/>
     </row>
-    <row r="302" spans="1:70" ht="182">
+    <row r="302" spans="1:70" ht="13" customHeight="1">
       <c r="A302" s="73" t="s">
         <v>46</v>
       </c>
@@ -29034,7 +29034,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="303" spans="1:70" ht="70">
+    <row r="303" spans="1:70" ht="13" customHeight="1">
       <c r="A303" s="73" t="s">
         <v>28</v>
       </c>
@@ -29088,7 +29088,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="304" spans="1:70" ht="98">
+    <row r="304" spans="1:70" ht="13" customHeight="1">
       <c r="A304" s="73" t="s">
         <v>46</v>
       </c>
@@ -29144,7 +29144,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="305" spans="1:70" ht="140">
+    <row r="305" spans="1:70" ht="13" customHeight="1">
       <c r="A305" s="73" t="s">
         <v>28</v>
       </c>
@@ -29193,7 +29193,7 @@
         <v>2203</v>
       </c>
     </row>
-    <row r="306" spans="1:70" s="78" customFormat="1">
+    <row r="306" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A306" s="77" t="s">
         <v>16</v>
       </c>
@@ -29235,7 +29235,7 @@
       <c r="X306" s="77"/>
       <c r="Y306" s="77"/>
     </row>
-    <row r="307" spans="1:70" s="78" customFormat="1" ht="98">
+    <row r="307" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A307" s="77" t="s">
         <v>291</v>
       </c>
@@ -29289,7 +29289,7 @@
       </c>
       <c r="Y307" s="77"/>
     </row>
-    <row r="308" spans="1:70" s="78" customFormat="1" ht="28">
+    <row r="308" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A308" s="77" t="s">
         <v>104</v>
       </c>
@@ -29329,7 +29329,7 @@
       <c r="X308" s="77"/>
       <c r="Y308" s="77"/>
     </row>
-    <row r="309" spans="1:70" s="78" customFormat="1">
+    <row r="309" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A309" s="77" t="s">
         <v>27</v>
       </c>
@@ -29363,7 +29363,7 @@
       <c r="X309" s="77"/>
       <c r="Y309" s="77"/>
     </row>
-    <row r="310" spans="1:70" s="78" customFormat="1" ht="84">
+    <row r="310" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A310" s="77" t="s">
         <v>20</v>
       </c>
@@ -29405,7 +29405,7 @@
       <c r="X310" s="73"/>
       <c r="Y310" s="77"/>
     </row>
-    <row r="311" spans="1:70" s="78" customFormat="1" ht="42">
+    <row r="311" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A311" s="77" t="s">
         <v>1030</v>
       </c>
@@ -29459,7 +29459,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="312" spans="1:70" s="78" customFormat="1" ht="140">
+    <row r="312" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A312" s="77" t="s">
         <v>200</v>
       </c>
@@ -29505,7 +29505,7 @@
       <c r="X312" s="77"/>
       <c r="Y312" s="77"/>
     </row>
-    <row r="313" spans="1:70" ht="409">
+    <row r="313" spans="1:70" ht="13" customHeight="1">
       <c r="A313" s="73" t="s">
         <v>16</v>
       </c>
@@ -29544,7 +29544,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="314" spans="1:70" s="74" customFormat="1" ht="98">
+    <row r="314" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A314" s="73" t="s">
         <v>20</v>
       </c>
@@ -29634,7 +29634,7 @@
       <c r="BQ314" s="75"/>
       <c r="BR314" s="75"/>
     </row>
-    <row r="315" spans="1:70" s="74" customFormat="1" ht="98">
+    <row r="315" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A315" s="73" t="s">
         <v>20</v>
       </c>
@@ -29724,7 +29724,7 @@
       <c r="BQ315" s="75"/>
       <c r="BR315" s="75"/>
     </row>
-    <row r="316" spans="1:70" s="74" customFormat="1" ht="56">
+    <row r="316" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A316" s="73" t="s">
         <v>20</v>
       </c>
@@ -29814,7 +29814,7 @@
       <c r="BQ316" s="75"/>
       <c r="BR316" s="75"/>
     </row>
-    <row r="317" spans="1:70" s="74" customFormat="1" ht="56">
+    <row r="317" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A317" s="73" t="s">
         <v>20</v>
       </c>
@@ -29904,7 +29904,7 @@
       <c r="BQ317" s="75"/>
       <c r="BR317" s="75"/>
     </row>
-    <row r="318" spans="1:70" ht="210">
+    <row r="318" spans="1:70" ht="13" customHeight="1">
       <c r="A318" s="73" t="s">
         <v>298</v>
       </c>
@@ -29953,7 +29953,7 @@
         <v>2205</v>
       </c>
     </row>
-    <row r="319" spans="1:70" ht="28">
+    <row r="319" spans="1:70" ht="13" customHeight="1">
       <c r="A319" s="73" t="s">
         <v>104</v>
       </c>
@@ -29992,7 +29992,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="320" spans="1:70">
+    <row r="320" spans="1:70" ht="13" customHeight="1">
       <c r="A320" s="73" t="s">
         <v>27</v>
       </c>
@@ -30024,7 +30024,7 @@
       </c>
       <c r="U320" s="75"/>
     </row>
-    <row r="321" spans="1:70" ht="70">
+    <row r="321" spans="1:70" ht="13" customHeight="1">
       <c r="A321" s="73" t="s">
         <v>825</v>
       </c>
@@ -30068,7 +30068,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="322" spans="1:70" s="78" customFormat="1" ht="56">
+    <row r="322" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A322" s="77" t="s">
         <v>200</v>
       </c>
@@ -30113,7 +30113,7 @@
       <c r="X322" s="77"/>
       <c r="Y322" s="77"/>
     </row>
-    <row r="323" spans="1:70" s="74" customFormat="1" ht="56">
+    <row r="323" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A323" s="73" t="s">
         <v>200</v>
       </c>
@@ -30209,7 +30209,7 @@
       <c r="BQ323" s="75"/>
       <c r="BR323" s="75"/>
     </row>
-    <row r="324" spans="1:70" s="74" customFormat="1" ht="56">
+    <row r="324" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A324" s="73" t="s">
         <v>200</v>
       </c>
@@ -30305,7 +30305,7 @@
       <c r="BQ324" s="75"/>
       <c r="BR324" s="75"/>
     </row>
-    <row r="325" spans="1:70" ht="56">
+    <row r="325" spans="1:70" ht="13" customHeight="1">
       <c r="A325" s="73" t="s">
         <v>200</v>
       </c>
@@ -30348,7 +30348,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="326" spans="1:70">
+    <row r="326" spans="1:70" ht="13" customHeight="1">
       <c r="A326" s="73" t="s">
         <v>16</v>
       </c>
@@ -30386,7 +30386,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="327" spans="1:70">
+    <row r="327" spans="1:70" ht="13" customHeight="1">
       <c r="A327" s="73" t="s">
         <v>20</v>
       </c>
@@ -30420,7 +30420,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="328" spans="1:70" ht="28">
+    <row r="328" spans="1:70" ht="13" customHeight="1">
       <c r="A328" s="73" t="s">
         <v>200</v>
       </c>
@@ -30451,7 +30451,7 @@
       </c>
       <c r="U328" s="75"/>
     </row>
-    <row r="329" spans="1:70" ht="28">
+    <row r="329" spans="1:70" ht="13" customHeight="1">
       <c r="A329" s="73" t="s">
         <v>200</v>
       </c>
@@ -30493,7 +30493,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="330" spans="1:70" ht="28">
+    <row r="330" spans="1:70" ht="13" customHeight="1">
       <c r="A330" s="73" t="s">
         <v>200</v>
       </c>
@@ -30535,7 +30535,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="331" spans="1:70" ht="42">
+    <row r="331" spans="1:70" ht="13" customHeight="1">
       <c r="A331" s="73" t="s">
         <v>200</v>
       </c>
@@ -30577,7 +30577,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="332" spans="1:70" s="78" customFormat="1" ht="42">
+    <row r="332" spans="1:70" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A332" s="77" t="s">
         <v>200</v>
       </c>
@@ -30622,7 +30622,7 @@
       <c r="X332" s="77"/>
       <c r="Y332" s="77"/>
     </row>
-    <row r="333" spans="1:70">
+    <row r="333" spans="1:70" ht="13" customHeight="1">
       <c r="A333" s="73" t="s">
         <v>27</v>
       </c>
@@ -30654,7 +30654,7 @@
       </c>
       <c r="U333" s="75"/>
     </row>
-    <row r="334" spans="1:70" s="85" customFormat="1" ht="154">
+    <row r="334" spans="1:70" s="85" customFormat="1" ht="13" customHeight="1">
       <c r="A334" s="84" t="s">
         <v>20</v>
       </c>
@@ -30702,7 +30702,7 @@
       <c r="X334" s="84"/>
       <c r="Y334" s="84"/>
     </row>
-    <row r="335" spans="1:70" s="85" customFormat="1" ht="168">
+    <row r="335" spans="1:70" s="85" customFormat="1" ht="13" customHeight="1">
       <c r="A335" s="84" t="s">
         <v>20</v>
       </c>
@@ -30746,7 +30746,7 @@
       <c r="X335" s="84"/>
       <c r="Y335" s="84"/>
     </row>
-    <row r="336" spans="1:70" ht="112">
+    <row r="336" spans="1:70" ht="13" customHeight="1">
       <c r="A336" s="73" t="s">
         <v>14</v>
       </c>
@@ -30780,7 +30780,7 @@
       </c>
       <c r="U336" s="75"/>
     </row>
-    <row r="337" spans="1:70" s="74" customFormat="1">
+    <row r="337" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A337" s="73" t="s">
         <v>16</v>
       </c>
@@ -30868,7 +30868,7 @@
       <c r="BQ337" s="75"/>
       <c r="BR337" s="75"/>
     </row>
-    <row r="338" spans="1:70" s="74" customFormat="1" ht="42">
+    <row r="338" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A338" s="73" t="s">
         <v>20</v>
       </c>
@@ -30956,7 +30956,7 @@
       <c r="BQ338" s="75"/>
       <c r="BR338" s="75"/>
     </row>
-    <row r="339" spans="1:70" s="74" customFormat="1">
+    <row r="339" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A339" s="73" t="s">
         <v>20</v>
       </c>
@@ -31040,7 +31040,7 @@
       <c r="BQ339" s="75"/>
       <c r="BR339" s="75"/>
     </row>
-    <row r="340" spans="1:70" s="74" customFormat="1" ht="28">
+    <row r="340" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A340" s="73" t="s">
         <v>20</v>
       </c>
@@ -31130,7 +31130,7 @@
       <c r="BQ340" s="75"/>
       <c r="BR340" s="75"/>
     </row>
-    <row r="341" spans="1:70" s="74" customFormat="1" ht="28">
+    <row r="341" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A341" s="73" t="s">
         <v>20</v>
       </c>
@@ -31220,7 +31220,7 @@
       <c r="BQ341" s="75"/>
       <c r="BR341" s="75"/>
     </row>
-    <row r="342" spans="1:70" s="74" customFormat="1" ht="140">
+    <row r="342" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A342" s="73" t="s">
         <v>46</v>
       </c>
@@ -31316,7 +31316,7 @@
       <c r="BQ342" s="75"/>
       <c r="BR342" s="75"/>
     </row>
-    <row r="343" spans="1:70" s="74" customFormat="1">
+    <row r="343" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A343" s="73" t="s">
         <v>27</v>
       </c>
@@ -31398,7 +31398,7 @@
       <c r="BQ343" s="75"/>
       <c r="BR343" s="75"/>
     </row>
-    <row r="344" spans="1:70" ht="98">
+    <row r="344" spans="1:70" ht="13" customHeight="1">
       <c r="A344" s="73" t="s">
         <v>20</v>
       </c>
@@ -31445,7 +31445,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="345" spans="1:70" ht="42">
+    <row r="345" spans="1:70" ht="13" customHeight="1">
       <c r="A345" s="73" t="s">
         <v>14</v>
       </c>
@@ -31482,7 +31482,7 @@
       </c>
       <c r="U345" s="75"/>
     </row>
-    <row r="346" spans="1:70" ht="98">
+    <row r="346" spans="1:70" ht="13" customHeight="1">
       <c r="A346" s="73" t="s">
         <v>28</v>
       </c>
@@ -31536,7 +31536,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="347" spans="1:70" ht="70">
+    <row r="347" spans="1:70" ht="13" customHeight="1">
       <c r="A347" s="73" t="s">
         <v>28</v>
       </c>
@@ -31594,7 +31594,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="348" spans="1:70" ht="84">
+    <row r="348" spans="1:70" ht="13" customHeight="1">
       <c r="A348" s="73" t="s">
         <v>28</v>
       </c>
@@ -31648,7 +31648,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="349" spans="1:70">
+    <row r="349" spans="1:70" ht="13" customHeight="1">
       <c r="A349" s="73" t="s">
         <v>14</v>
       </c>
@@ -31685,7 +31685,7 @@
       </c>
       <c r="U349" s="75"/>
     </row>
-    <row r="350" spans="1:70" s="74" customFormat="1" ht="84">
+    <row r="350" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A350" s="75" t="s">
         <v>16</v>
       </c>
@@ -31773,7 +31773,7 @@
       <c r="BQ350" s="75"/>
       <c r="BR350" s="75"/>
     </row>
-    <row r="351" spans="1:70" ht="28">
+    <row r="351" spans="1:70" ht="13" customHeight="1">
       <c r="A351" s="75" t="s">
         <v>20</v>
       </c>
@@ -31800,7 +31800,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="352" spans="1:70" s="74" customFormat="1" ht="42">
+    <row r="352" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A352" s="75" t="s">
         <v>20</v>
       </c>
@@ -31888,7 +31888,7 @@
       <c r="BQ352" s="75"/>
       <c r="BR352" s="75"/>
     </row>
-    <row r="353" spans="1:70" s="74" customFormat="1" ht="42">
+    <row r="353" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A353" s="75" t="s">
         <v>20</v>
       </c>
@@ -31976,7 +31976,7 @@
       <c r="BQ353" s="75"/>
       <c r="BR353" s="75"/>
     </row>
-    <row r="354" spans="1:70" s="74" customFormat="1" ht="238">
+    <row r="354" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A354" s="75" t="s">
         <v>1450</v>
       </c>
@@ -32074,7 +32074,7 @@
       <c r="BQ354" s="75"/>
       <c r="BR354" s="75"/>
     </row>
-    <row r="355" spans="1:70" s="74" customFormat="1">
+    <row r="355" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A355" s="75" t="s">
         <v>27</v>
       </c>
@@ -32156,7 +32156,7 @@
       <c r="BQ355" s="75"/>
       <c r="BR355" s="75"/>
     </row>
-    <row r="356" spans="1:70" s="99" customFormat="1" ht="98">
+    <row r="356" spans="1:70" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A356" s="75" t="s">
         <v>14</v>
       </c>
@@ -32240,7 +32240,7 @@
       <c r="BQ356" s="77"/>
       <c r="BR356" s="77"/>
     </row>
-    <row r="357" spans="1:70" s="90" customFormat="1" ht="210">
+    <row r="357" spans="1:70" s="90" customFormat="1" ht="13" customHeight="1">
       <c r="A357" s="75" t="s">
         <v>46</v>
       </c>
@@ -32342,7 +32342,7 @@
       <c r="BQ357" s="78"/>
       <c r="BR357" s="78"/>
     </row>
-    <row r="358" spans="1:70" s="90" customFormat="1" ht="294">
+    <row r="358" spans="1:70" s="90" customFormat="1" ht="13" customHeight="1">
       <c r="A358" s="75" t="s">
         <v>14</v>
       </c>
@@ -32422,7 +32422,7 @@
       <c r="BQ358" s="78"/>
       <c r="BR358" s="78"/>
     </row>
-    <row r="359" spans="1:70" s="74" customFormat="1" ht="238">
+    <row r="359" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A359" s="75" t="s">
         <v>20</v>
       </c>
@@ -32480,7 +32480,7 @@
       <c r="AK359" s="75"/>
       <c r="AL359" s="75"/>
     </row>
-    <row r="360" spans="1:70" s="74" customFormat="1" ht="350">
+    <row r="360" spans="1:70" s="74" customFormat="1" ht="13" customHeight="1">
       <c r="A360" s="75" t="s">
         <v>20</v>
       </c>
@@ -32538,7 +32538,7 @@
       <c r="AK360" s="75"/>
       <c r="AL360" s="75"/>
     </row>
-    <row r="361" spans="1:70" s="108" customFormat="1" ht="168">
+    <row r="361" spans="1:70" s="108" customFormat="1" ht="13" customHeight="1">
       <c r="A361" s="83" t="s">
         <v>1131</v>
       </c>
@@ -32602,7 +32602,7 @@
       <c r="AK361" s="82"/>
       <c r="AL361" s="82"/>
     </row>
-    <row r="362" spans="1:70" s="108" customFormat="1" ht="98">
+    <row r="362" spans="1:70" s="108" customFormat="1" ht="13" customHeight="1">
       <c r="A362" s="83" t="s">
         <v>14</v>
       </c>
@@ -32654,7 +32654,7 @@
       <c r="AK362" s="82"/>
       <c r="AL362" s="82"/>
     </row>
-    <row r="363" spans="1:70" s="108" customFormat="1" ht="28">
+    <row r="363" spans="1:70" s="108" customFormat="1" ht="13" customHeight="1">
       <c r="A363" s="83" t="s">
         <v>46</v>
       </c>
@@ -32716,7 +32716,7 @@
       <c r="AK363" s="82"/>
       <c r="AL363" s="82"/>
     </row>
-    <row r="364" spans="1:70" s="108" customFormat="1" ht="168">
+    <row r="364" spans="1:70" s="108" customFormat="1" ht="13" customHeight="1">
       <c r="A364" s="83" t="s">
         <v>1131</v>
       </c>
@@ -32780,7 +32780,7 @@
       <c r="AK364" s="82"/>
       <c r="AL364" s="82"/>
     </row>
-    <row r="365" spans="1:70" s="108" customFormat="1" ht="98">
+    <row r="365" spans="1:70" s="108" customFormat="1" ht="13" customHeight="1">
       <c r="A365" s="83" t="s">
         <v>14</v>
       </c>
@@ -32832,7 +32832,7 @@
       <c r="AK365" s="82"/>
       <c r="AL365" s="82"/>
     </row>
-    <row r="366" spans="1:70" s="108" customFormat="1" ht="28">
+    <row r="366" spans="1:70" s="108" customFormat="1" ht="13" customHeight="1">
       <c r="A366" s="83" t="s">
         <v>46</v>
       </c>
@@ -32894,7 +32894,7 @@
       <c r="AK366" s="82"/>
       <c r="AL366" s="82"/>
     </row>
-    <row r="367" spans="1:70" s="99" customFormat="1" ht="196">
+    <row r="367" spans="1:70" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A367" s="77" t="s">
         <v>16</v>
       </c>
@@ -32948,7 +32948,7 @@
       <c r="AK367" s="77"/>
       <c r="AL367" s="77"/>
     </row>
-    <row r="368" spans="1:70" s="112" customFormat="1" ht="308">
+    <row r="368" spans="1:70" s="112" customFormat="1" ht="13" customHeight="1">
       <c r="A368" s="76" t="s">
         <v>20</v>
       </c>
@@ -33010,7 +33010,7 @@
       <c r="AK368" s="76"/>
       <c r="AL368" s="76"/>
     </row>
-    <row r="369" spans="1:38" s="99" customFormat="1" ht="56">
+    <row r="369" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A369" s="77" t="s">
         <v>1070</v>
       </c>
@@ -33068,7 +33068,7 @@
       <c r="AK369" s="77"/>
       <c r="AL369" s="77"/>
     </row>
-    <row r="370" spans="1:38" s="99" customFormat="1" ht="112">
+    <row r="370" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A370" s="77" t="s">
         <v>14</v>
       </c>
@@ -33120,7 +33120,7 @@
       <c r="AK370" s="77"/>
       <c r="AL370" s="77"/>
     </row>
-    <row r="371" spans="1:38" s="99" customFormat="1" ht="84">
+    <row r="371" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A371" s="77" t="s">
         <v>1073</v>
       </c>
@@ -33190,7 +33190,7 @@
       <c r="AK371" s="77"/>
       <c r="AL371" s="77"/>
     </row>
-    <row r="372" spans="1:38" s="99" customFormat="1" ht="70">
+    <row r="372" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A372" s="77" t="s">
         <v>1078</v>
       </c>
@@ -33258,7 +33258,7 @@
       <c r="AK372" s="77"/>
       <c r="AL372" s="77"/>
     </row>
-    <row r="373" spans="1:38" s="99" customFormat="1" ht="112">
+    <row r="373" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A373" s="77" t="s">
         <v>200</v>
       </c>
@@ -33318,7 +33318,7 @@
       <c r="AK373" s="77"/>
       <c r="AL373" s="77"/>
     </row>
-    <row r="374" spans="1:38" s="99" customFormat="1" ht="70">
+    <row r="374" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A374" s="77" t="s">
         <v>200</v>
       </c>
@@ -33378,7 +33378,7 @@
       <c r="AK374" s="77"/>
       <c r="AL374" s="77"/>
     </row>
-    <row r="375" spans="1:38" s="77" customFormat="1" ht="409">
+    <row r="375" spans="1:38" s="77" customFormat="1" ht="13" customHeight="1">
       <c r="A375" s="77" t="s">
         <v>14</v>
       </c>
@@ -33403,7 +33403,7 @@
       <c r="X375" s="73"/>
       <c r="Y375" s="73"/>
     </row>
-    <row r="376" spans="1:38" s="77" customFormat="1" ht="224">
+    <row r="376" spans="1:38" s="77" customFormat="1" ht="13" customHeight="1">
       <c r="A376" s="77" t="s">
         <v>1084</v>
       </c>
@@ -33446,7 +33446,7 @@
       <c r="X376" s="73"/>
       <c r="Y376" s="73"/>
     </row>
-    <row r="377" spans="1:38" ht="42">
+    <row r="377" spans="1:38" ht="13" customHeight="1">
       <c r="A377" s="75" t="s">
         <v>200</v>
       </c>
@@ -33476,7 +33476,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="378" spans="1:38" s="99" customFormat="1" ht="56">
+    <row r="378" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A378" s="75" t="s">
         <v>200</v>
       </c>
@@ -33536,7 +33536,7 @@
       <c r="AK378" s="77"/>
       <c r="AL378" s="77"/>
     </row>
-    <row r="379" spans="1:38" s="99" customFormat="1" ht="42">
+    <row r="379" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A379" s="75" t="s">
         <v>200</v>
       </c>
@@ -33596,7 +33596,7 @@
       <c r="AK379" s="77"/>
       <c r="AL379" s="77"/>
     </row>
-    <row r="380" spans="1:38" s="99" customFormat="1" ht="56">
+    <row r="380" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A380" s="75" t="s">
         <v>200</v>
       </c>
@@ -33656,7 +33656,7 @@
       <c r="AK380" s="77"/>
       <c r="AL380" s="77"/>
     </row>
-    <row r="381" spans="1:38" s="99" customFormat="1">
+    <row r="381" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A381" s="77" t="s">
         <v>27</v>
       </c>
@@ -33706,7 +33706,7 @@
       <c r="AK381" s="77"/>
       <c r="AL381" s="77"/>
     </row>
-    <row r="382" spans="1:38" s="99" customFormat="1" ht="112">
+    <row r="382" spans="1:38" s="99" customFormat="1" ht="13" customHeight="1">
       <c r="A382" s="77" t="s">
         <v>46</v>
       </c>
@@ -33772,7 +33772,7 @@
       <c r="AK382" s="77"/>
       <c r="AL382" s="77"/>
     </row>
-    <row r="383" spans="1:38" s="119" customFormat="1">
+    <row r="383" spans="1:38" s="119" customFormat="1" ht="13" customHeight="1">
       <c r="A383" s="117" t="s">
         <v>20</v>
       </c>
@@ -33812,7 +33812,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="384" spans="1:38" ht="112">
+    <row r="384" spans="1:38" ht="13" customHeight="1">
       <c r="A384" s="75" t="s">
         <v>200</v>
       </c>
@@ -33848,7 +33848,7 @@
       <c r="X384" s="75"/>
       <c r="Y384" s="75"/>
     </row>
-    <row r="385" spans="1:25" ht="28">
+    <row r="385" spans="1:25" ht="13" customHeight="1">
       <c r="A385" s="75" t="s">
         <v>200</v>
       </c>
@@ -33884,7 +33884,7 @@
       <c r="X385" s="75"/>
       <c r="Y385" s="75"/>
     </row>
-    <row r="386" spans="1:25" ht="168">
+    <row r="386" spans="1:25" ht="13" customHeight="1">
       <c r="A386" s="75" t="s">
         <v>37</v>
       </c>
@@ -33931,7 +33931,7 @@
       <c r="X386" s="75"/>
       <c r="Y386" s="75"/>
     </row>
-    <row r="387" spans="1:25" ht="56">
+    <row r="387" spans="1:25" ht="13" customHeight="1">
       <c r="A387" s="75" t="s">
         <v>28</v>
       </c>
@@ -33980,7 +33980,7 @@
       </c>
       <c r="Y387" s="75"/>
     </row>
-    <row r="388" spans="1:25" ht="154">
+    <row r="388" spans="1:25" ht="13" customHeight="1">
       <c r="A388" s="73" t="s">
         <v>20</v>
       </c>
@@ -34027,7 +34027,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="389" spans="1:25" ht="98">
+    <row r="389" spans="1:25" ht="13" customHeight="1">
       <c r="A389" s="73" t="s">
         <v>20</v>
       </c>
@@ -34076,7 +34076,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="390" spans="1:25" s="120" customFormat="1" ht="28">
+    <row r="390" spans="1:25" s="120" customFormat="1" ht="13" customHeight="1">
       <c r="A390" s="120" t="s">
         <v>20</v>
       </c>
@@ -34099,7 +34099,7 @@
       <c r="W390" s="121"/>
       <c r="X390" s="121"/>
     </row>
-    <row r="391" spans="1:25" ht="168">
+    <row r="391" spans="1:25" ht="13" customHeight="1">
       <c r="A391" s="73" t="s">
         <v>342</v>
       </c>
@@ -34143,7 +34143,7 @@
         <v>2688</v>
       </c>
     </row>
-    <row r="392" spans="1:25" ht="42">
+    <row r="392" spans="1:25" ht="13" customHeight="1">
       <c r="A392" s="73" t="s">
         <v>345</v>
       </c>
@@ -34187,7 +34187,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="393" spans="1:25" s="78" customFormat="1" ht="28">
+    <row r="393" spans="1:25" s="78" customFormat="1" ht="13" customHeight="1">
       <c r="A393" s="77" t="s">
         <v>962</v>
       </c>
@@ -34233,7 +34233,7 @@
       <c r="X393" s="77"/>
       <c r="Y393" s="77"/>
     </row>
-    <row r="394" spans="1:25" s="82" customFormat="1">
+    <row r="394" spans="1:25" s="82" customFormat="1" ht="13" customHeight="1">
       <c r="A394" s="83" t="s">
         <v>16</v>
       </c>
@@ -34273,7 +34273,7 @@
       <c r="X394" s="83"/>
       <c r="Y394" s="83"/>
     </row>
-    <row r="395" spans="1:25" s="82" customFormat="1" ht="56">
+    <row r="395" spans="1:25" s="82" customFormat="1" ht="13" customHeight="1">
       <c r="A395" s="83" t="s">
         <v>20</v>
       </c>
@@ -34315,7 +34315,7 @@
       <c r="X395" s="83"/>
       <c r="Y395" s="83"/>
     </row>
-    <row r="396" spans="1:25" s="82" customFormat="1" ht="28">
+    <row r="396" spans="1:25" s="82" customFormat="1" ht="13" customHeight="1">
       <c r="A396" s="83" t="s">
         <v>1195</v>
       </c>
@@ -34353,7 +34353,7 @@
       <c r="X396" s="83"/>
       <c r="Y396" s="83"/>
     </row>
-    <row r="397" spans="1:25" s="82" customFormat="1" ht="28">
+    <row r="397" spans="1:25" s="82" customFormat="1" ht="13" customHeight="1">
       <c r="A397" s="83" t="s">
         <v>1195</v>
       </c>
@@ -34391,7 +34391,7 @@
       <c r="X397" s="83"/>
       <c r="Y397" s="83"/>
     </row>
-    <row r="398" spans="1:25" s="82" customFormat="1" ht="28">
+    <row r="398" spans="1:25" s="82" customFormat="1" ht="13" customHeight="1">
       <c r="A398" s="83" t="s">
         <v>1195</v>
       </c>
@@ -34429,7 +34429,7 @@
       <c r="X398" s="83"/>
       <c r="Y398" s="83"/>
     </row>
-    <row r="399" spans="1:25" s="82" customFormat="1" ht="28">
+    <row r="399" spans="1:25" s="82" customFormat="1" ht="13" customHeight="1">
       <c r="A399" s="83" t="s">
         <v>1195</v>
       </c>
@@ -34467,7 +34467,7 @@
       <c r="X399" s="83"/>
       <c r="Y399" s="83"/>
     </row>
-    <row r="400" spans="1:25" s="82" customFormat="1">
+    <row r="400" spans="1:25" s="82" customFormat="1" ht="13" customHeight="1">
       <c r="A400" s="83" t="s">
         <v>27</v>
       </c>
@@ -34501,7 +34501,7 @@
       <c r="X400" s="83"/>
       <c r="Y400" s="83"/>
     </row>
-    <row r="401" spans="1:25" ht="84">
+    <row r="401" spans="1:25" ht="13" customHeight="1">
       <c r="A401" s="73" t="s">
         <v>347</v>
       </c>
@@ -34556,7 +34556,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="402" spans="1:25">
+    <row r="402" spans="1:25" ht="13" customHeight="1">
       <c r="A402" s="73" t="s">
         <v>352</v>
       </c>
@@ -34586,7 +34586,7 @@
       </c>
       <c r="U402" s="75"/>
     </row>
-    <row r="403" spans="1:25">
+    <row r="403" spans="1:25" ht="13" customHeight="1">
       <c r="A403" s="73" t="s">
         <v>353</v>
       </c>
@@ -34616,7 +34616,7 @@
       </c>
       <c r="U403" s="75"/>
     </row>
-    <row r="404" spans="1:25">
+    <row r="404" spans="1:25" ht="13" customHeight="1">
       <c r="A404" s="73" t="s">
         <v>354</v>
       </c>
@@ -34646,7 +34646,7 @@
       </c>
       <c r="U404" s="75"/>
     </row>
-    <row r="405" spans="1:25">
+    <row r="405" spans="1:25" ht="13" customHeight="1">
       <c r="A405" s="73" t="s">
         <v>355</v>
       </c>
@@ -34676,7 +34676,7 @@
       </c>
       <c r="U405" s="75"/>
     </row>
-    <row r="406" spans="1:25">
+    <row r="406" spans="1:25" ht="13" customHeight="1">
       <c r="A406" s="73" t="s">
         <v>356</v>
       </c>
@@ -34706,7 +34706,7 @@
       </c>
       <c r="U406" s="75"/>
     </row>
-    <row r="407" spans="1:25" s="115" customFormat="1">
+    <row r="407" spans="1:25" s="115" customFormat="1" ht="13" customHeight="1">
       <c r="A407" s="114" t="s">
         <v>968</v>
       </c>
@@ -34738,7 +34738,7 @@
       <c r="X407" s="114"/>
       <c r="Y407" s="114"/>
     </row>
-    <row r="408" spans="1:25" s="115" customFormat="1">
+    <row r="408" spans="1:25" s="115" customFormat="1" ht="13" customHeight="1">
       <c r="A408" s="114" t="s">
         <v>970</v>
       </c>
@@ -34770,7 +34770,7 @@
       <c r="X408" s="114"/>
       <c r="Y408" s="114"/>
     </row>
-    <row r="409" spans="1:25" s="115" customFormat="1" ht="28">
+    <row r="409" spans="1:25" s="115" customFormat="1" ht="13" customHeight="1">
       <c r="A409" s="114" t="s">
         <v>968</v>
       </c>
@@ -34806,7 +34806,7 @@
       <c r="X409" s="114"/>
       <c r="Y409" s="114"/>
     </row>
-    <row r="410" spans="1:25" s="115" customFormat="1">
+    <row r="410" spans="1:25" s="115" customFormat="1" ht="13" customHeight="1">
       <c r="A410" s="114"/>
       <c r="B410" s="114"/>
       <c r="C410" s="114"/>
@@ -34830,842 +34830,842 @@
       <c r="X410" s="114"/>
       <c r="Y410" s="114"/>
     </row>
-    <row r="411" spans="1:25">
+    <row r="411" spans="1:25" ht="13" customHeight="1">
       <c r="P411" s="75"/>
       <c r="S411" s="75"/>
       <c r="U411" s="75"/>
     </row>
-    <row r="412" spans="1:25">
+    <row r="412" spans="1:25" ht="13" customHeight="1">
       <c r="P412" s="75"/>
       <c r="S412" s="75"/>
       <c r="U412" s="75"/>
     </row>
-    <row r="413" spans="1:25">
+    <row r="413" spans="1:25" ht="13" customHeight="1">
       <c r="P413" s="75"/>
       <c r="S413" s="75"/>
       <c r="U413" s="75"/>
     </row>
-    <row r="414" spans="1:25">
+    <row r="414" spans="1:25" ht="13" customHeight="1">
       <c r="P414" s="75"/>
       <c r="S414" s="75"/>
       <c r="U414" s="75"/>
     </row>
-    <row r="415" spans="1:25">
+    <row r="415" spans="1:25" ht="13" customHeight="1">
       <c r="P415" s="75"/>
       <c r="S415" s="75"/>
       <c r="U415" s="75"/>
     </row>
-    <row r="416" spans="1:25">
+    <row r="416" spans="1:25" ht="13" customHeight="1">
       <c r="P416" s="75"/>
       <c r="S416" s="75"/>
       <c r="U416" s="75"/>
     </row>
-    <row r="417" spans="16:21">
+    <row r="417" spans="16:21" ht="13" customHeight="1">
       <c r="P417" s="75"/>
       <c r="S417" s="75"/>
       <c r="U417" s="75"/>
     </row>
-    <row r="418" spans="16:21">
+    <row r="418" spans="16:21" ht="13" customHeight="1">
       <c r="P418" s="75"/>
       <c r="S418" s="75"/>
       <c r="U418" s="75"/>
     </row>
-    <row r="419" spans="16:21">
+    <row r="419" spans="16:21" ht="13" customHeight="1">
       <c r="P419" s="75"/>
       <c r="S419" s="75"/>
       <c r="U419" s="75"/>
     </row>
-    <row r="420" spans="16:21">
+    <row r="420" spans="16:21" ht="13" customHeight="1">
       <c r="P420" s="75"/>
       <c r="S420" s="75"/>
       <c r="U420" s="75"/>
     </row>
-    <row r="421" spans="16:21">
+    <row r="421" spans="16:21" ht="13" customHeight="1">
       <c r="P421" s="75"/>
       <c r="S421" s="75"/>
       <c r="U421" s="75"/>
     </row>
-    <row r="422" spans="16:21">
+    <row r="422" spans="16:21" ht="13" customHeight="1">
       <c r="P422" s="75"/>
       <c r="S422" s="75"/>
       <c r="U422" s="75"/>
     </row>
-    <row r="423" spans="16:21">
+    <row r="423" spans="16:21" ht="13" customHeight="1">
       <c r="P423" s="75"/>
       <c r="S423" s="75"/>
       <c r="U423" s="75"/>
     </row>
-    <row r="424" spans="16:21">
+    <row r="424" spans="16:21" ht="13" customHeight="1">
       <c r="P424" s="75"/>
       <c r="S424" s="75"/>
       <c r="U424" s="75"/>
     </row>
-    <row r="425" spans="16:21">
+    <row r="425" spans="16:21" ht="13" customHeight="1">
       <c r="P425" s="75"/>
       <c r="S425" s="75"/>
       <c r="U425" s="75"/>
     </row>
-    <row r="426" spans="16:21">
+    <row r="426" spans="16:21" ht="13" customHeight="1">
       <c r="P426" s="75"/>
       <c r="S426" s="75"/>
       <c r="U426" s="75"/>
     </row>
-    <row r="427" spans="16:21">
+    <row r="427" spans="16:21" ht="13" customHeight="1">
       <c r="P427" s="75"/>
       <c r="S427" s="75"/>
       <c r="U427" s="75"/>
     </row>
-    <row r="428" spans="16:21">
+    <row r="428" spans="16:21" ht="13" customHeight="1">
       <c r="P428" s="75"/>
       <c r="S428" s="75"/>
       <c r="U428" s="75"/>
     </row>
-    <row r="429" spans="16:21">
+    <row r="429" spans="16:21" ht="13" customHeight="1">
       <c r="P429" s="75"/>
       <c r="S429" s="75"/>
       <c r="U429" s="75"/>
     </row>
-    <row r="430" spans="16:21">
+    <row r="430" spans="16:21" ht="13" customHeight="1">
       <c r="P430" s="75"/>
       <c r="S430" s="75"/>
       <c r="U430" s="75"/>
     </row>
-    <row r="431" spans="16:21">
+    <row r="431" spans="16:21" ht="13" customHeight="1">
       <c r="P431" s="75"/>
       <c r="S431" s="75"/>
       <c r="U431" s="75"/>
     </row>
-    <row r="432" spans="16:21">
+    <row r="432" spans="16:21" ht="13" customHeight="1">
       <c r="P432" s="75"/>
       <c r="S432" s="75"/>
       <c r="U432" s="75"/>
     </row>
-    <row r="433" spans="16:21">
+    <row r="433" spans="16:21" ht="13" customHeight="1">
       <c r="P433" s="75"/>
       <c r="S433" s="75"/>
       <c r="U433" s="75"/>
     </row>
-    <row r="434" spans="16:21">
+    <row r="434" spans="16:21" ht="13" customHeight="1">
       <c r="P434" s="75"/>
       <c r="S434" s="75"/>
       <c r="U434" s="75"/>
     </row>
-    <row r="435" spans="16:21">
+    <row r="435" spans="16:21" ht="13" customHeight="1">
       <c r="P435" s="75"/>
       <c r="S435" s="75"/>
       <c r="U435" s="75"/>
     </row>
-    <row r="436" spans="16:21">
+    <row r="436" spans="16:21" ht="13" customHeight="1">
       <c r="P436" s="75"/>
       <c r="S436" s="75"/>
       <c r="U436" s="75"/>
     </row>
-    <row r="437" spans="16:21">
+    <row r="437" spans="16:21" ht="13" customHeight="1">
       <c r="P437" s="75"/>
       <c r="S437" s="75"/>
       <c r="U437" s="75"/>
     </row>
-    <row r="438" spans="16:21">
+    <row r="438" spans="16:21" ht="13" customHeight="1">
       <c r="P438" s="75"/>
       <c r="S438" s="75"/>
       <c r="U438" s="75"/>
     </row>
-    <row r="439" spans="16:21">
+    <row r="439" spans="16:21" ht="13" customHeight="1">
       <c r="P439" s="75"/>
       <c r="S439" s="75"/>
       <c r="U439" s="75"/>
     </row>
-    <row r="440" spans="16:21">
+    <row r="440" spans="16:21" ht="13" customHeight="1">
       <c r="P440" s="75"/>
       <c r="S440" s="75"/>
       <c r="U440" s="75"/>
     </row>
-    <row r="441" spans="16:21">
+    <row r="441" spans="16:21" ht="13" customHeight="1">
       <c r="P441" s="75"/>
       <c r="S441" s="75"/>
       <c r="U441" s="75"/>
     </row>
-    <row r="442" spans="16:21">
+    <row r="442" spans="16:21" ht="13" customHeight="1">
       <c r="P442" s="75"/>
       <c r="S442" s="75"/>
       <c r="U442" s="75"/>
     </row>
-    <row r="443" spans="16:21">
+    <row r="443" spans="16:21" ht="13" customHeight="1">
       <c r="P443" s="75"/>
       <c r="S443" s="75"/>
       <c r="U443" s="75"/>
     </row>
-    <row r="444" spans="16:21">
+    <row r="444" spans="16:21" ht="13" customHeight="1">
       <c r="P444" s="75"/>
       <c r="S444" s="75"/>
       <c r="U444" s="75"/>
     </row>
-    <row r="445" spans="16:21">
+    <row r="445" spans="16:21" ht="13" customHeight="1">
       <c r="P445" s="75"/>
       <c r="S445" s="75"/>
       <c r="U445" s="75"/>
     </row>
-    <row r="446" spans="16:21">
+    <row r="446" spans="16:21" ht="13" customHeight="1">
       <c r="P446" s="75"/>
       <c r="S446" s="75"/>
       <c r="U446" s="75"/>
     </row>
-    <row r="447" spans="16:21">
+    <row r="447" spans="16:21" ht="13" customHeight="1">
       <c r="P447" s="75"/>
       <c r="S447" s="75"/>
       <c r="U447" s="75"/>
     </row>
-    <row r="448" spans="16:21">
+    <row r="448" spans="16:21" ht="13" customHeight="1">
       <c r="P448" s="75"/>
       <c r="S448" s="75"/>
       <c r="U448" s="75"/>
     </row>
-    <row r="449" spans="16:21">
+    <row r="449" spans="16:21" ht="13" customHeight="1">
       <c r="P449" s="75"/>
       <c r="S449" s="75"/>
       <c r="U449" s="75"/>
     </row>
-    <row r="450" spans="16:21">
+    <row r="450" spans="16:21" ht="13" customHeight="1">
       <c r="P450" s="75"/>
       <c r="S450" s="75"/>
       <c r="U450" s="75"/>
     </row>
-    <row r="451" spans="16:21">
+    <row r="451" spans="16:21" ht="13" customHeight="1">
       <c r="P451" s="75"/>
       <c r="S451" s="75"/>
       <c r="U451" s="75"/>
     </row>
-    <row r="452" spans="16:21">
+    <row r="452" spans="16:21" ht="13" customHeight="1">
       <c r="P452" s="75"/>
       <c r="S452" s="75"/>
       <c r="U452" s="75"/>
     </row>
-    <row r="453" spans="16:21">
+    <row r="453" spans="16:21" ht="13" customHeight="1">
       <c r="P453" s="75"/>
       <c r="S453" s="75"/>
       <c r="U453" s="75"/>
     </row>
-    <row r="454" spans="16:21">
+    <row r="454" spans="16:21" ht="13" customHeight="1">
       <c r="P454" s="75"/>
       <c r="S454" s="75"/>
       <c r="U454" s="75"/>
     </row>
-    <row r="455" spans="16:21">
+    <row r="455" spans="16:21" ht="13" customHeight="1">
       <c r="P455" s="75"/>
       <c r="S455" s="75"/>
       <c r="U455" s="75"/>
     </row>
-    <row r="456" spans="16:21">
+    <row r="456" spans="16:21" ht="13" customHeight="1">
       <c r="P456" s="75"/>
       <c r="S456" s="75"/>
       <c r="U456" s="75"/>
     </row>
-    <row r="457" spans="16:21">
+    <row r="457" spans="16:21" ht="13" customHeight="1">
       <c r="P457" s="75"/>
       <c r="S457" s="75"/>
       <c r="U457" s="75"/>
     </row>
-    <row r="458" spans="16:21">
+    <row r="458" spans="16:21" ht="13" customHeight="1">
       <c r="P458" s="75"/>
       <c r="S458" s="75"/>
       <c r="U458" s="75"/>
     </row>
-    <row r="459" spans="16:21">
+    <row r="459" spans="16:21" ht="13" customHeight="1">
       <c r="P459" s="75"/>
       <c r="S459" s="75"/>
       <c r="U459" s="75"/>
     </row>
-    <row r="460" spans="16:21">
+    <row r="460" spans="16:21" ht="13" customHeight="1">
       <c r="P460" s="75"/>
       <c r="S460" s="75"/>
       <c r="U460" s="75"/>
     </row>
-    <row r="461" spans="16:21">
+    <row r="461" spans="16:21" ht="13" customHeight="1">
       <c r="P461" s="75"/>
       <c r="S461" s="75"/>
       <c r="U461" s="75"/>
     </row>
-    <row r="462" spans="16:21">
+    <row r="462" spans="16:21" ht="13" customHeight="1">
       <c r="P462" s="75"/>
       <c r="S462" s="75"/>
       <c r="U462" s="75"/>
     </row>
-    <row r="463" spans="16:21">
+    <row r="463" spans="16:21" ht="13" customHeight="1">
       <c r="P463" s="75"/>
       <c r="S463" s="75"/>
       <c r="U463" s="75"/>
     </row>
-    <row r="464" spans="16:21">
+    <row r="464" spans="16:21" ht="13" customHeight="1">
       <c r="P464" s="75"/>
       <c r="S464" s="75"/>
       <c r="U464" s="75"/>
     </row>
-    <row r="465" spans="16:21">
+    <row r="465" spans="16:21" ht="13" customHeight="1">
       <c r="P465" s="75"/>
       <c r="S465" s="75"/>
       <c r="U465" s="75"/>
     </row>
-    <row r="466" spans="16:21">
+    <row r="466" spans="16:21" ht="13" customHeight="1">
       <c r="P466" s="75"/>
       <c r="S466" s="75"/>
       <c r="U466" s="75"/>
     </row>
-    <row r="467" spans="16:21">
+    <row r="467" spans="16:21" ht="13" customHeight="1">
       <c r="P467" s="75"/>
       <c r="S467" s="75"/>
       <c r="U467" s="75"/>
     </row>
-    <row r="468" spans="16:21">
+    <row r="468" spans="16:21" ht="13" customHeight="1">
       <c r="P468" s="75"/>
       <c r="S468" s="75"/>
       <c r="U468" s="75"/>
     </row>
-    <row r="469" spans="16:21">
+    <row r="469" spans="16:21" ht="13" customHeight="1">
       <c r="P469" s="75"/>
       <c r="S469" s="75"/>
       <c r="U469" s="75"/>
     </row>
-    <row r="470" spans="16:21">
+    <row r="470" spans="16:21" ht="13" customHeight="1">
       <c r="P470" s="75"/>
       <c r="S470" s="75"/>
       <c r="U470" s="75"/>
     </row>
-    <row r="471" spans="16:21">
+    <row r="471" spans="16:21" ht="13" customHeight="1">
       <c r="P471" s="75"/>
       <c r="S471" s="75"/>
       <c r="U471" s="75"/>
     </row>
-    <row r="472" spans="16:21">
+    <row r="472" spans="16:21" ht="13" customHeight="1">
       <c r="P472" s="75"/>
       <c r="S472" s="75"/>
       <c r="U472" s="75"/>
     </row>
-    <row r="473" spans="16:21">
+    <row r="473" spans="16:21" ht="13" customHeight="1">
       <c r="P473" s="75"/>
       <c r="S473" s="75"/>
       <c r="U473" s="75"/>
     </row>
-    <row r="474" spans="16:21">
+    <row r="474" spans="16:21" ht="13" customHeight="1">
       <c r="P474" s="75"/>
       <c r="S474" s="75"/>
       <c r="U474" s="75"/>
     </row>
-    <row r="475" spans="16:21">
+    <row r="475" spans="16:21" ht="13" customHeight="1">
       <c r="P475" s="75"/>
       <c r="S475" s="75"/>
       <c r="U475" s="75"/>
     </row>
-    <row r="476" spans="16:21">
+    <row r="476" spans="16:21" ht="13" customHeight="1">
       <c r="P476" s="75"/>
       <c r="S476" s="75"/>
       <c r="U476" s="75"/>
     </row>
-    <row r="477" spans="16:21">
+    <row r="477" spans="16:21" ht="13" customHeight="1">
       <c r="P477" s="75"/>
       <c r="S477" s="75"/>
       <c r="U477" s="75"/>
     </row>
-    <row r="478" spans="16:21">
+    <row r="478" spans="16:21" ht="13" customHeight="1">
       <c r="P478" s="75"/>
       <c r="S478" s="75"/>
       <c r="U478" s="75"/>
     </row>
-    <row r="479" spans="16:21">
+    <row r="479" spans="16:21" ht="13" customHeight="1">
       <c r="P479" s="75"/>
       <c r="S479" s="75"/>
       <c r="U479" s="75"/>
     </row>
-    <row r="480" spans="16:21">
+    <row r="480" spans="16:21" ht="13" customHeight="1">
       <c r="P480" s="75"/>
       <c r="S480" s="75"/>
       <c r="U480" s="75"/>
     </row>
-    <row r="481" spans="16:21">
+    <row r="481" spans="16:21" ht="13" customHeight="1">
       <c r="P481" s="75"/>
       <c r="S481" s="75"/>
       <c r="U481" s="75"/>
     </row>
-    <row r="482" spans="16:21">
+    <row r="482" spans="16:21" ht="13" customHeight="1">
       <c r="P482" s="75"/>
       <c r="S482" s="75"/>
       <c r="U482" s="75"/>
     </row>
-    <row r="483" spans="16:21">
+    <row r="483" spans="16:21" ht="13" customHeight="1">
       <c r="P483" s="75"/>
       <c r="S483" s="75"/>
       <c r="U483" s="75"/>
     </row>
-    <row r="484" spans="16:21">
+    <row r="484" spans="16:21" ht="13" customHeight="1">
       <c r="P484" s="75"/>
       <c r="S484" s="75"/>
       <c r="U484" s="75"/>
     </row>
-    <row r="485" spans="16:21">
+    <row r="485" spans="16:21" ht="13" customHeight="1">
       <c r="P485" s="75"/>
       <c r="S485" s="75"/>
       <c r="U485" s="75"/>
     </row>
-    <row r="486" spans="16:21">
+    <row r="486" spans="16:21" ht="13" customHeight="1">
       <c r="P486" s="75"/>
       <c r="S486" s="75"/>
       <c r="U486" s="75"/>
     </row>
-    <row r="487" spans="16:21">
+    <row r="487" spans="16:21" ht="13" customHeight="1">
       <c r="P487" s="75"/>
       <c r="S487" s="75"/>
       <c r="U487" s="75"/>
     </row>
-    <row r="488" spans="16:21">
+    <row r="488" spans="16:21" ht="13" customHeight="1">
       <c r="P488" s="75"/>
       <c r="S488" s="75"/>
       <c r="U488" s="75"/>
     </row>
-    <row r="489" spans="16:21">
+    <row r="489" spans="16:21" ht="13" customHeight="1">
       <c r="P489" s="75"/>
       <c r="S489" s="75"/>
       <c r="U489" s="75"/>
     </row>
-    <row r="490" spans="16:21">
+    <row r="490" spans="16:21" ht="13" customHeight="1">
       <c r="P490" s="75"/>
       <c r="S490" s="75"/>
       <c r="U490" s="75"/>
     </row>
-    <row r="491" spans="16:21">
+    <row r="491" spans="16:21" ht="13" customHeight="1">
       <c r="P491" s="75"/>
       <c r="S491" s="75"/>
       <c r="U491" s="75"/>
     </row>
-    <row r="492" spans="16:21">
+    <row r="492" spans="16:21" ht="13" customHeight="1">
       <c r="P492" s="75"/>
       <c r="S492" s="75"/>
       <c r="U492" s="75"/>
     </row>
-    <row r="493" spans="16:21">
+    <row r="493" spans="16:21" ht="13" customHeight="1">
       <c r="P493" s="75"/>
       <c r="S493" s="75"/>
       <c r="U493" s="75"/>
     </row>
-    <row r="494" spans="16:21">
+    <row r="494" spans="16:21" ht="13" customHeight="1">
       <c r="P494" s="75"/>
       <c r="S494" s="75"/>
       <c r="U494" s="75"/>
     </row>
-    <row r="495" spans="16:21">
+    <row r="495" spans="16:21" ht="13" customHeight="1">
       <c r="P495" s="75"/>
       <c r="S495" s="75"/>
       <c r="U495" s="75"/>
     </row>
-    <row r="496" spans="16:21">
+    <row r="496" spans="16:21" ht="13" customHeight="1">
       <c r="P496" s="75"/>
       <c r="S496" s="75"/>
       <c r="U496" s="75"/>
     </row>
-    <row r="497" spans="16:21">
+    <row r="497" spans="16:21" ht="13" customHeight="1">
       <c r="P497" s="75"/>
       <c r="S497" s="75"/>
       <c r="U497" s="75"/>
     </row>
-    <row r="498" spans="16:21">
+    <row r="498" spans="16:21" ht="13" customHeight="1">
       <c r="P498" s="75"/>
       <c r="S498" s="75"/>
       <c r="U498" s="75"/>
     </row>
-    <row r="499" spans="16:21">
+    <row r="499" spans="16:21" ht="13" customHeight="1">
       <c r="P499" s="75"/>
       <c r="S499" s="75"/>
       <c r="U499" s="75"/>
     </row>
-    <row r="500" spans="16:21">
+    <row r="500" spans="16:21" ht="13" customHeight="1">
       <c r="P500" s="75"/>
       <c r="S500" s="75"/>
       <c r="U500" s="75"/>
     </row>
-    <row r="501" spans="16:21">
+    <row r="501" spans="16:21" ht="13" customHeight="1">
       <c r="P501" s="75"/>
       <c r="S501" s="75"/>
       <c r="U501" s="75"/>
     </row>
-    <row r="502" spans="16:21">
+    <row r="502" spans="16:21" ht="13" customHeight="1">
       <c r="P502" s="75"/>
       <c r="S502" s="75"/>
       <c r="U502" s="75"/>
     </row>
-    <row r="503" spans="16:21">
+    <row r="503" spans="16:21" ht="13" customHeight="1">
       <c r="P503" s="75"/>
       <c r="S503" s="75"/>
       <c r="U503" s="75"/>
     </row>
-    <row r="504" spans="16:21">
+    <row r="504" spans="16:21" ht="13" customHeight="1">
       <c r="P504" s="75"/>
       <c r="S504" s="75"/>
       <c r="U504" s="75"/>
     </row>
-    <row r="505" spans="16:21">
+    <row r="505" spans="16:21" ht="13" customHeight="1">
       <c r="P505" s="75"/>
       <c r="S505" s="75"/>
       <c r="U505" s="75"/>
     </row>
-    <row r="506" spans="16:21">
+    <row r="506" spans="16:21" ht="13" customHeight="1">
       <c r="P506" s="75"/>
       <c r="S506" s="75"/>
       <c r="U506" s="75"/>
     </row>
-    <row r="507" spans="16:21">
+    <row r="507" spans="16:21" ht="13" customHeight="1">
       <c r="P507" s="75"/>
       <c r="S507" s="75"/>
       <c r="U507" s="75"/>
     </row>
-    <row r="508" spans="16:21">
+    <row r="508" spans="16:21" ht="13" customHeight="1">
       <c r="P508" s="75"/>
       <c r="S508" s="75"/>
       <c r="U508" s="75"/>
     </row>
-    <row r="509" spans="16:21">
+    <row r="509" spans="16:21" ht="13" customHeight="1">
       <c r="P509" s="75"/>
       <c r="S509" s="75"/>
       <c r="U509" s="75"/>
     </row>
-    <row r="510" spans="16:21">
+    <row r="510" spans="16:21" ht="13" customHeight="1">
       <c r="P510" s="75"/>
       <c r="S510" s="75"/>
       <c r="U510" s="75"/>
     </row>
-    <row r="511" spans="16:21">
+    <row r="511" spans="16:21" ht="13" customHeight="1">
       <c r="P511" s="75"/>
       <c r="S511" s="75"/>
       <c r="U511" s="75"/>
     </row>
-    <row r="512" spans="16:21">
+    <row r="512" spans="16:21" ht="13" customHeight="1">
       <c r="P512" s="75"/>
       <c r="S512" s="75"/>
       <c r="U512" s="75"/>
     </row>
-    <row r="513" spans="16:21">
+    <row r="513" spans="16:21" ht="13" customHeight="1">
       <c r="P513" s="75"/>
       <c r="S513" s="75"/>
       <c r="U513" s="75"/>
     </row>
-    <row r="514" spans="16:21">
+    <row r="514" spans="16:21" ht="13" customHeight="1">
       <c r="P514" s="75"/>
       <c r="S514" s="75"/>
       <c r="U514" s="75"/>
     </row>
-    <row r="515" spans="16:21">
+    <row r="515" spans="16:21" ht="13" customHeight="1">
       <c r="P515" s="75"/>
       <c r="S515" s="75"/>
       <c r="U515" s="75"/>
     </row>
-    <row r="516" spans="16:21">
+    <row r="516" spans="16:21" ht="13" customHeight="1">
       <c r="P516" s="75"/>
       <c r="S516" s="75"/>
       <c r="U516" s="75"/>
     </row>
-    <row r="517" spans="16:21">
+    <row r="517" spans="16:21" ht="13" customHeight="1">
       <c r="P517" s="75"/>
       <c r="S517" s="75"/>
       <c r="U517" s="75"/>
     </row>
-    <row r="518" spans="16:21">
+    <row r="518" spans="16:21" ht="13" customHeight="1">
       <c r="P518" s="75"/>
       <c r="S518" s="75"/>
       <c r="U518" s="75"/>
     </row>
-    <row r="519" spans="16:21">
+    <row r="519" spans="16:21" ht="13" customHeight="1">
       <c r="P519" s="75"/>
       <c r="S519" s="75"/>
       <c r="U519" s="75"/>
     </row>
-    <row r="520" spans="16:21">
+    <row r="520" spans="16:21" ht="13" customHeight="1">
       <c r="P520" s="75"/>
       <c r="S520" s="75"/>
       <c r="U520" s="75"/>
     </row>
-    <row r="521" spans="16:21">
+    <row r="521" spans="16:21" ht="13" customHeight="1">
       <c r="P521" s="75"/>
       <c r="S521" s="75"/>
       <c r="U521" s="75"/>
     </row>
-    <row r="522" spans="16:21">
+    <row r="522" spans="16:21" ht="13" customHeight="1">
       <c r="P522" s="75"/>
       <c r="S522" s="75"/>
       <c r="U522" s="75"/>
     </row>
-    <row r="523" spans="16:21">
+    <row r="523" spans="16:21" ht="13" customHeight="1">
       <c r="P523" s="75"/>
       <c r="S523" s="75"/>
       <c r="U523" s="75"/>
     </row>
-    <row r="524" spans="16:21">
+    <row r="524" spans="16:21" ht="13" customHeight="1">
       <c r="P524" s="75"/>
       <c r="S524" s="75"/>
       <c r="U524" s="75"/>
     </row>
-    <row r="525" spans="16:21">
+    <row r="525" spans="16:21" ht="13" customHeight="1">
       <c r="P525" s="75"/>
       <c r="S525" s="75"/>
       <c r="U525" s="75"/>
     </row>
-    <row r="526" spans="16:21">
+    <row r="526" spans="16:21" ht="13" customHeight="1">
       <c r="P526" s="75"/>
       <c r="S526" s="75"/>
       <c r="U526" s="75"/>
     </row>
-    <row r="527" spans="16:21">
+    <row r="527" spans="16:21" ht="13" customHeight="1">
       <c r="P527" s="75"/>
       <c r="S527" s="75"/>
       <c r="U527" s="75"/>
     </row>
-    <row r="528" spans="16:21">
+    <row r="528" spans="16:21" ht="13" customHeight="1">
       <c r="P528" s="75"/>
       <c r="S528" s="75"/>
       <c r="U528" s="75"/>
     </row>
-    <row r="529" spans="16:21">
+    <row r="529" spans="16:21" ht="13" customHeight="1">
       <c r="P529" s="75"/>
       <c r="S529" s="75"/>
       <c r="U529" s="75"/>
     </row>
-    <row r="530" spans="16:21">
+    <row r="530" spans="16:21" ht="13" customHeight="1">
       <c r="P530" s="75"/>
       <c r="S530" s="75"/>
       <c r="U530" s="75"/>
     </row>
-    <row r="531" spans="16:21">
+    <row r="531" spans="16:21" ht="13" customHeight="1">
       <c r="P531" s="75"/>
       <c r="S531" s="75"/>
       <c r="U531" s="75"/>
     </row>
-    <row r="532" spans="16:21">
+    <row r="532" spans="16:21" ht="13" customHeight="1">
       <c r="P532" s="75"/>
       <c r="S532" s="75"/>
       <c r="U532" s="75"/>
     </row>
-    <row r="533" spans="16:21">
+    <row r="533" spans="16:21" ht="13" customHeight="1">
       <c r="P533" s="75"/>
       <c r="S533" s="75"/>
       <c r="U533" s="75"/>
     </row>
-    <row r="534" spans="16:21">
+    <row r="534" spans="16:21" ht="13" customHeight="1">
       <c r="P534" s="75"/>
       <c r="S534" s="75"/>
       <c r="U534" s="75"/>
     </row>
-    <row r="535" spans="16:21">
+    <row r="535" spans="16:21" ht="13" customHeight="1">
       <c r="P535" s="75"/>
       <c r="S535" s="75"/>
       <c r="U535" s="75"/>
     </row>
-    <row r="536" spans="16:21">
+    <row r="536" spans="16:21" ht="13" customHeight="1">
       <c r="P536" s="75"/>
       <c r="S536" s="75"/>
       <c r="U536" s="75"/>
     </row>
-    <row r="537" spans="16:21">
+    <row r="537" spans="16:21" ht="13" customHeight="1">
       <c r="P537" s="75"/>
       <c r="S537" s="75"/>
       <c r="U537" s="75"/>
     </row>
-    <row r="538" spans="16:21">
+    <row r="538" spans="16:21" ht="13" customHeight="1">
       <c r="P538" s="75"/>
       <c r="S538" s="75"/>
       <c r="U538" s="75"/>
     </row>
-    <row r="539" spans="16:21">
+    <row r="539" spans="16:21" ht="13" customHeight="1">
       <c r="P539" s="75"/>
       <c r="S539" s="75"/>
       <c r="U539" s="75"/>
     </row>
-    <row r="540" spans="16:21">
+    <row r="540" spans="16:21" ht="13" customHeight="1">
       <c r="P540" s="75"/>
       <c r="S540" s="75"/>
       <c r="U540" s="75"/>
     </row>
-    <row r="541" spans="16:21">
+    <row r="541" spans="16:21" ht="13" customHeight="1">
       <c r="P541" s="75"/>
       <c r="S541" s="75"/>
       <c r="U541" s="75"/>
     </row>
-    <row r="542" spans="16:21">
+    <row r="542" spans="16:21" ht="13" customHeight="1">
       <c r="P542" s="75"/>
       <c r="S542" s="75"/>
       <c r="U542" s="75"/>
     </row>
-    <row r="543" spans="16:21">
+    <row r="543" spans="16:21" ht="13" customHeight="1">
       <c r="P543" s="75"/>
       <c r="S543" s="75"/>
       <c r="U543" s="75"/>
     </row>
-    <row r="544" spans="16:21">
+    <row r="544" spans="16:21" ht="13" customHeight="1">
       <c r="P544" s="75"/>
       <c r="S544" s="75"/>
       <c r="U544" s="75"/>
     </row>
-    <row r="545" spans="16:21">
+    <row r="545" spans="16:21" ht="13" customHeight="1">
       <c r="P545" s="75"/>
       <c r="S545" s="75"/>
       <c r="U545" s="75"/>
     </row>
-    <row r="546" spans="16:21">
+    <row r="546" spans="16:21" ht="13" customHeight="1">
       <c r="P546" s="75"/>
       <c r="S546" s="75"/>
       <c r="U546" s="75"/>
     </row>
-    <row r="547" spans="16:21">
+    <row r="547" spans="16:21" ht="13" customHeight="1">
       <c r="P547" s="75"/>
       <c r="S547" s="75"/>
       <c r="U547" s="75"/>
     </row>
-    <row r="548" spans="16:21">
+    <row r="548" spans="16:21" ht="13" customHeight="1">
       <c r="P548" s="75"/>
       <c r="S548" s="75"/>
       <c r="U548" s="75"/>
     </row>
-    <row r="549" spans="16:21">
+    <row r="549" spans="16:21" ht="13" customHeight="1">
       <c r="P549" s="75"/>
       <c r="S549" s="75"/>
       <c r="U549" s="75"/>
     </row>
-    <row r="550" spans="16:21">
+    <row r="550" spans="16:21" ht="13" customHeight="1">
       <c r="P550" s="75"/>
       <c r="S550" s="75"/>
       <c r="U550" s="75"/>
     </row>
-    <row r="551" spans="16:21">
+    <row r="551" spans="16:21" ht="13" customHeight="1">
       <c r="P551" s="75"/>
       <c r="S551" s="75"/>
       <c r="U551" s="75"/>
     </row>
-    <row r="552" spans="16:21">
+    <row r="552" spans="16:21" ht="13" customHeight="1">
       <c r="P552" s="75"/>
       <c r="S552" s="75"/>
       <c r="U552" s="75"/>
     </row>
-    <row r="553" spans="16:21">
+    <row r="553" spans="16:21" ht="13" customHeight="1">
       <c r="P553" s="75"/>
       <c r="S553" s="75"/>
       <c r="U553" s="75"/>
     </row>
-    <row r="554" spans="16:21">
+    <row r="554" spans="16:21" ht="13" customHeight="1">
       <c r="P554" s="75"/>
       <c r="S554" s="75"/>
       <c r="U554" s="75"/>
     </row>
-    <row r="555" spans="16:21">
+    <row r="555" spans="16:21" ht="13" customHeight="1">
       <c r="P555" s="75"/>
       <c r="S555" s="75"/>
       <c r="U555" s="75"/>
     </row>
-    <row r="556" spans="16:21">
+    <row r="556" spans="16:21" ht="13" customHeight="1">
       <c r="P556" s="75"/>
       <c r="S556" s="75"/>
       <c r="U556" s="75"/>
     </row>
-    <row r="557" spans="16:21">
+    <row r="557" spans="16:21" ht="13" customHeight="1">
       <c r="P557" s="75"/>
       <c r="S557" s="75"/>
       <c r="U557" s="75"/>
     </row>
-    <row r="558" spans="16:21">
+    <row r="558" spans="16:21" ht="13" customHeight="1">
       <c r="P558" s="75"/>
       <c r="S558" s="75"/>
       <c r="U558" s="75"/>
     </row>
-    <row r="559" spans="16:21">
+    <row r="559" spans="16:21" ht="13" customHeight="1">
       <c r="P559" s="75"/>
       <c r="S559" s="75"/>
       <c r="U559" s="75"/>
     </row>
-    <row r="560" spans="16:21">
+    <row r="560" spans="16:21" ht="13" customHeight="1">
       <c r="P560" s="75"/>
       <c r="S560" s="75"/>
       <c r="U560" s="75"/>
     </row>
-    <row r="561" spans="16:21">
+    <row r="561" spans="16:21" ht="13" customHeight="1">
       <c r="P561" s="75"/>
       <c r="S561" s="75"/>
       <c r="U561" s="75"/>
     </row>
-    <row r="562" spans="16:21">
+    <row r="562" spans="16:21" ht="13" customHeight="1">
       <c r="P562" s="75"/>
       <c r="S562" s="75"/>
       <c r="U562" s="75"/>
     </row>
-    <row r="563" spans="16:21">
+    <row r="563" spans="16:21" ht="13" customHeight="1">
       <c r="P563" s="75"/>
       <c r="S563" s="75"/>
       <c r="U563" s="75"/>
     </row>
-    <row r="564" spans="16:21">
+    <row r="564" spans="16:21" ht="13" customHeight="1">
       <c r="P564" s="75"/>
       <c r="S564" s="75"/>
       <c r="U564" s="75"/>
     </row>
-    <row r="565" spans="16:21">
+    <row r="565" spans="16:21" ht="13" customHeight="1">
       <c r="P565" s="75"/>
       <c r="S565" s="75"/>
       <c r="U565" s="75"/>
     </row>
-    <row r="566" spans="16:21">
+    <row r="566" spans="16:21" ht="13" customHeight="1">
       <c r="P566" s="75"/>
       <c r="S566" s="75"/>
       <c r="U566" s="75"/>
     </row>
-    <row r="567" spans="16:21">
+    <row r="567" spans="16:21" ht="13" customHeight="1">
       <c r="P567" s="75"/>
       <c r="S567" s="75"/>
       <c r="U567" s="75"/>
     </row>
-    <row r="568" spans="16:21">
+    <row r="568" spans="16:21" ht="13" customHeight="1">
       <c r="P568" s="75"/>
       <c r="S568" s="75"/>
       <c r="U568" s="75"/>
     </row>
-    <row r="569" spans="16:21">
+    <row r="569" spans="16:21" ht="13" customHeight="1">
       <c r="P569" s="75"/>
       <c r="S569" s="75"/>
       <c r="U569" s="75"/>
     </row>
-    <row r="570" spans="16:21">
+    <row r="570" spans="16:21" ht="13" customHeight="1">
       <c r="P570" s="75"/>
       <c r="S570" s="75"/>
       <c r="U570" s="75"/>
     </row>
-    <row r="571" spans="16:21">
+    <row r="571" spans="16:21" ht="13" customHeight="1">
       <c r="P571" s="75"/>
       <c r="S571" s="75"/>
       <c r="U571" s="75"/>
     </row>
-    <row r="572" spans="16:21">
+    <row r="572" spans="16:21" ht="13" customHeight="1">
       <c r="P572" s="75"/>
       <c r="S572" s="75"/>
       <c r="U572" s="75"/>
     </row>
-    <row r="573" spans="16:21">
+    <row r="573" spans="16:21" ht="13" customHeight="1">
       <c r="P573" s="75"/>
       <c r="S573" s="75"/>
       <c r="U573" s="75"/>
     </row>
-    <row r="574" spans="16:21">
+    <row r="574" spans="16:21" ht="13" customHeight="1">
       <c r="P574" s="75"/>
       <c r="S574" s="75"/>
       <c r="U574" s="75"/>
     </row>
-    <row r="575" spans="16:21">
+    <row r="575" spans="16:21" ht="13" customHeight="1">
       <c r="P575" s="75"/>
       <c r="S575" s="75"/>
       <c r="U575" s="75"/>
     </row>
-    <row r="576" spans="16:21">
+    <row r="576" spans="16:21" ht="13" customHeight="1">
       <c r="P576" s="75"/>
       <c r="S576" s="75"/>
       <c r="U576" s="75"/>
     </row>
-    <row r="577" spans="16:21">
+    <row r="577" spans="16:21" ht="13" customHeight="1">
       <c r="P577" s="75"/>
       <c r="S577" s="75"/>
       <c r="U577" s="75"/>
     </row>
-    <row r="578" spans="16:21">
+    <row r="578" spans="16:21" ht="13" customHeight="1">
       <c r="P578" s="75"/>
       <c r="S578" s="75"/>
       <c r="U578" s="75"/>
@@ -40645,7 +40645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>

</xml_diff>